<commit_message>
pgd debug voltages 1e-4 errors
</commit_message>
<xml_diff>
--- a/Initial presentation/Codi/PGD/Map_I.xlsx
+++ b/Initial presentation/Codi/PGD/Map_I.xlsx
@@ -26,1819 +26,1819 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="605">
   <si>
-    <t>(1.520994357196908e-05+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05622531106540892+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11383807663300659+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11508975092988644+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11621778278477327+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11720315484627584+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11804281040911498+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11872342562113364+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11924253428955336+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11958843563230415+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11976659800404858+0j)</t>
-  </si>
-  <si>
-    <t>(-2.7895356320639144e-07+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05630765165030448+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11384327473437161+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11513113120324366+0j)</t>
-  </si>
-  <si>
-    <t>(-0.1161968239533718+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11724453661049329+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11811074744053089+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11869478751615195+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11922986526754607+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11951917540246242+0j)</t>
-  </si>
-  <si>
-    <t>(-0.1197328047860344+0j)</t>
-  </si>
-  <si>
-    <t>(3.134168821102383e-05+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05626862069579134+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11387320330385081+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11513865805607487+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11625022943727988+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11724500797776315+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11807795682989623+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11873715912251508+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11924441067444762+0j)</t>
-  </si>
-  <si>
-    <t>(-0.1195815374967622+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11975023823089802+0j)</t>
-  </si>
-  <si>
-    <t>(4.0338973998774055e-05+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0562716735775157+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11389998800673794+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11515084247726637+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11626589107998755+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11723917735672215+0j)</t>
-  </si>
-  <si>
-    <t>(-0.1180563306470447+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11872813003433984+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11922285802757825+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11956844247507892+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11972328893828475+0j)</t>
-  </si>
-  <si>
-    <t>(3.504904795627547e-05+0j)</t>
-  </si>
-  <si>
-    <t>(-0.056301104241168805+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11390799346793318+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11515986065378893+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11624726245808097+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11722660940783348+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11803737554596676+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11867133393368043+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11915650522059412+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11948054455943527+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11963501811410743+0j)</t>
-  </si>
-  <si>
-    <t>(6.0816424026723474e-06+0j)</t>
-  </si>
-  <si>
-    <t>(-0.056277293056530384+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11390210164333629+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11514352748097018+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11624706777673936+0j)</t>
-  </si>
-  <si>
-    <t>(-0.1172186664583+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11803794504774319+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11869571517820914+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11919663927420854+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11953147571965882+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11969919364667336+0j)</t>
-  </si>
-  <si>
-    <t>(0.016986358502878628+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0489805873850887+0j)</t>
-  </si>
-  <si>
-    <t>(-0.10600689902316236+0j)</t>
-  </si>
-  <si>
-    <t>(-0.10422318930432056+0j)</t>
-  </si>
-  <si>
-    <t>(-0.10682406868042141+0j)</t>
-  </si>
-  <si>
-    <t>(-0.10217419556081049+0j)</t>
-  </si>
-  <si>
-    <t>(-0.09838103522758103+0j)</t>
-  </si>
-  <si>
-    <t>(-0.10266550466570674+0j)</t>
-  </si>
-  <si>
-    <t>(-0.09903724657703211+0j)</t>
-  </si>
-  <si>
-    <t>(-0.10192570650717832+0j)</t>
-  </si>
-  <si>
-    <t>(-0.09736447396175128+0j)</t>
-  </si>
-  <si>
-    <t>(0.03365047800316243+0j)</t>
-  </si>
-  <si>
-    <t>(-0.04199048162793154+0j)</t>
-  </si>
-  <si>
-    <t>(-0.09848411595370615+0j)</t>
-  </si>
-  <si>
-    <t>(-0.09385085242921797+0j)</t>
-  </si>
-  <si>
-    <t>(-0.09791413162215183+0j)</t>
-  </si>
-  <si>
-    <t>(-0.08794028917777919+0j)</t>
-  </si>
-  <si>
-    <t>(-0.07978380510880673+0j)</t>
-  </si>
-  <si>
-    <t>(-0.08754165012649225+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0800006650850329+0j)</t>
-  </si>
-  <si>
-    <t>(-0.08532943679713052+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0762748988877007+0j)</t>
-  </si>
-  <si>
-    <t>(0.05005124312042039+0j)</t>
-  </si>
-  <si>
-    <t>(-0.03523315045202937+0j)</t>
-  </si>
-  <si>
-    <t>(-0.09129559152468895+0j)</t>
-  </si>
-  <si>
-    <t>(-0.08394843051729621+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0894697525273556+0j)</t>
-  </si>
-  <si>
-    <t>(-0.07439943112031806+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0620811507716104+0j)</t>
-  </si>
-  <si>
-    <t>(-0.07321641613933286+0j)</t>
-  </si>
-  <si>
-    <t>(-0.061940840486429075+0j)</t>
-  </si>
-  <si>
-    <t>(-0.06963220055160768+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05627362382834421+0j)</t>
-  </si>
-  <si>
-    <t>(0.0662272916545023+0j)</t>
-  </si>
-  <si>
-    <t>(-0.02867527008356797+0j)</t>
-  </si>
-  <si>
-    <t>(-0.08439790367443177+0j)</t>
-  </si>
-  <si>
-    <t>(-0.07445543694752109+0j)</t>
-  </si>
-  <si>
-    <t>(-0.08143327996844635+0j)</t>
-  </si>
-  <si>
-    <t>(-0.06146844966068768+0j)</t>
-  </si>
-  <si>
-    <t>(-0.04517034376644294+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05960019684097266+0j)</t>
-  </si>
-  <si>
-    <t>(-0.04475232129559952+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05473765419074897+0j)</t>
-  </si>
-  <si>
-    <t>(-0.037247339866546436+0j)</t>
-  </si>
-  <si>
-    <t>(-3.0645571255830565e-06+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0562841049339874+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11391162812977111+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11515159958778148+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11625357452225815+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11722476817764971+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11804455997438197+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11870218595137076+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11920487350214896+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11953962864811873+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11970955970622521+0j)</t>
-  </si>
-  <si>
-    <t>(0.03363646928058799+0j)</t>
-  </si>
-  <si>
-    <t>(-0.041976723708144426+0j)</t>
-  </si>
-  <si>
-    <t>(-0.09851040469522813+0j)</t>
-  </si>
-  <si>
-    <t>(-0.09385953519269506+0j)</t>
-  </si>
-  <si>
-    <t>(-0.09794035637593515+0j)</t>
-  </si>
-  <si>
-    <t>(-0.08793800037662651+0j)</t>
-  </si>
-  <si>
-    <t>(-0.07976652343196851+0j)</t>
-  </si>
-  <si>
-    <t>(-0.08755480909959763+0j)</t>
-  </si>
-  <si>
-    <t>(-0.08000446648381959+0j)</t>
-  </si>
-  <si>
-    <t>(-0.08535093641986233+0j)</t>
-  </si>
-  <si>
-    <t>(-0.07628272065046934+0j)</t>
-  </si>
-  <si>
-    <t>(0.06625200234016755+0j)</t>
-  </si>
-  <si>
-    <t>(-0.028703100039367116+0j)</t>
-  </si>
-  <si>
-    <t>(-0.08444060057668334+0j)</t>
-  </si>
-  <si>
-    <t>(-0.074455094882449+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0814035343344426+0j)</t>
-  </si>
-  <si>
-    <t>(-0.061432952167509956+0j)</t>
-  </si>
-  <si>
-    <t>(-0.04515227470001985+0j)</t>
-  </si>
-  <si>
-    <t>(-0.059556299057165196+0j)</t>
-  </si>
-  <si>
-    <t>(-0.04474245098006891+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05470451695549023+0j)</t>
-  </si>
-  <si>
-    <t>(-0.037263968759645265+0j)</t>
-  </si>
-  <si>
-    <t>(0.09800471038317021+0j)</t>
-  </si>
-  <si>
-    <t>(-0.016198040037882618+0j)</t>
-  </si>
-  <si>
-    <t>(-0.07140481535681989+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05649102622386165+0j)</t>
-  </si>
-  <si>
-    <t>(-0.06624458482644928+0j)</t>
-  </si>
-  <si>
-    <t>(-0.03703644071333423+0j)</t>
-  </si>
-  <si>
-    <t>(-0.013296288704325664+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0339628129682091+0j)</t>
-  </si>
-  <si>
-    <t>(-0.012469880255975518+0j)</t>
-  </si>
-  <si>
-    <t>(-0.026769954626712958+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0015927362887075064+0j)</t>
-  </si>
-  <si>
-    <t>(0.1290191882263536+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0042958656308896325+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05917819100468296+0j)</t>
-  </si>
-  <si>
-    <t>(-0.03965589964549434+0j)</t>
-  </si>
-  <si>
-    <t>(-0.052167509187982505+0j)</t>
-  </si>
-  <si>
-    <t>(-0.01429608484931646+0j)</t>
-  </si>
-  <si>
-    <t>(0.01639167003220787+0j)</t>
-  </si>
-  <si>
-    <t>(-0.01026368509364609+0j)</t>
-  </si>
-  <si>
-    <t>(0.017447007509650093+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0009752670864592681+0j)</t>
-  </si>
-  <si>
-    <t>(0.03143790827974477+0j)</t>
-  </si>
-  <si>
-    <t>(-8.874403611585316e-06+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05628118911385663+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11390711725325889+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11514664371182674+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11625020231273256+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11722260907922737+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11804529441783236+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11870575886351391+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11921212854000252+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11954829811681056+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11972122688540934+0j)</t>
-  </si>
-  <si>
-    <t>(0.0500421273690783+0j)</t>
-  </si>
-  <si>
-    <t>(-0.03522991952493074+0j)</t>
-  </si>
-  <si>
-    <t>(-0.09133342724841093+0j)</t>
-  </si>
-  <si>
-    <t>(-0.08395947383697665+0j)</t>
-  </si>
-  <si>
-    <t>(-0.08948898191616739+0j)</t>
-  </si>
-  <si>
-    <t>(-0.07439242303467161+0j)</t>
-  </si>
-  <si>
-    <t>(-0.062066680954184335+0j)</t>
-  </si>
-  <si>
-    <t>(-0.07322278507326666+0j)</t>
-  </si>
-  <si>
-    <t>(-0.06194964789292491+0j)</t>
-  </si>
-  <si>
-    <t>(-0.06965076517606268+0j)</t>
-  </si>
-  <si>
-    <t>(-0.056294989370872704+0j)</t>
-  </si>
-  <si>
-    <t>(0.09801741654367237+0j)</t>
-  </si>
-  <si>
-    <t>(-0.016199233603280454+0j)</t>
-  </si>
-  <si>
-    <t>(-0.07142779591684931+0j)</t>
-  </si>
-  <si>
-    <t>(-0.056498800771986234+0j)</t>
-  </si>
-  <si>
-    <t>(-0.06625415270200219+0j)</t>
-  </si>
-  <si>
-    <t>(-0.03703371661592644+0j)</t>
-  </si>
-  <si>
-    <t>(-0.013291294449098432+0j)</t>
-  </si>
-  <si>
-    <t>(-0.03396529288258145+0j)</t>
-  </si>
-  <si>
-    <t>(-0.012475465813000002+0j)</t>
-  </si>
-  <si>
-    <t>(-0.026778247347774366+0j)</t>
-  </si>
-  <si>
-    <t>(-0.001605354685511758+0j)</t>
-  </si>
-  <si>
-    <t>(0.14430588890792384+0j)</t>
-  </si>
-  <si>
-    <t>(0.0013823442218995207+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05339505555223542+0j)</t>
-  </si>
-  <si>
-    <t>(-0.03164053027272214+0j)</t>
-  </si>
-  <si>
-    <t>(-0.04545471709406198+0j)</t>
-  </si>
-  <si>
-    <t>(-0.003452446509810654+0j)</t>
-  </si>
-  <si>
-    <t>(0.030523482095336108+0j)</t>
-  </si>
-  <si>
-    <t>(0.0010339361564693358+0j)</t>
-  </si>
-  <si>
-    <t>(0.03167329355115392+0j)</t>
-  </si>
-  <si>
-    <t>(0.011308686491546007+0j)</t>
-  </si>
-  <si>
-    <t>(0.04712204026944315+0j)</t>
-  </si>
-  <si>
-    <t>(0.18917348081167482+0j)</t>
-  </si>
-  <si>
-    <t>(0.017874320332652256+0j)</t>
-  </si>
-  <si>
-    <t>(-0.036748992442437706+0j)</t>
-  </si>
-  <si>
-    <t>(-0.008714790930826805+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0264578214742763+0j)</t>
-  </si>
-  <si>
-    <t>(0.02732778644834453+0j)</t>
-  </si>
-  <si>
-    <t>(0.07066187459159942+0j)</t>
-  </si>
-  <si>
-    <t>(0.032881763272052986+0j)</t>
-  </si>
-  <si>
-    <t>(0.0718820846479019+0j)</t>
-  </si>
-  <si>
-    <t>(0.04585654227815718+0j)</t>
-  </si>
-  <si>
-    <t>(0.0914407479784407+0j)</t>
-  </si>
-  <si>
-    <t>(-1.0925078736106354e-05+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05627798952659737+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11390126633736972+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11513965356316322+0j)</t>
-  </si>
-  <si>
-    <t>(-0.1162437639183483+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11721621246163966+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11804002750709378+0j)</t>
-  </si>
-  <si>
-    <t>(-0.1187021751892758+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11921020618558498+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11954728965473793+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11972145421549245+0j)</t>
-  </si>
-  <si>
-    <t>(0.06623297438264367+0j)</t>
-  </si>
-  <si>
-    <t>(-0.02870277531421402+0j)</t>
-  </si>
-  <si>
-    <t>(-0.08444504759179947+0j)</t>
-  </si>
-  <si>
-    <t>(-0.07446329097556142+0j)</t>
-  </si>
-  <si>
-    <t>(-0.08141837846149214+0j)</t>
-  </si>
-  <si>
-    <t>(-0.06144047900979515+0j)</t>
-  </si>
-  <si>
-    <t>(-0.045149878816216314+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05956494349451051+0j)</t>
-  </si>
-  <si>
-    <t>(-0.044739961123137766+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05471094964569728+0j)</t>
-  </si>
-  <si>
-    <t>(-0.03725546896724359+0j)</t>
-  </si>
-  <si>
-    <t>(0.12905486121610638+0j)</t>
-  </si>
-  <si>
-    <t>(-0.004337490051229764+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05923989680213471+0j)</t>
-  </si>
-  <si>
-    <t>(-0.039689582496742495+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05217425076789816+0j)</t>
-  </si>
-  <si>
-    <t>(-0.014300291720769544+0j)</t>
-  </si>
-  <si>
-    <t>(0.01637826334597631+0j)</t>
-  </si>
-  <si>
-    <t>(-0.010249774060322986+0j)</t>
-  </si>
-  <si>
-    <t>(0.01744167978778274+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0009595445741949498+0j)</t>
-  </si>
-  <si>
-    <t>(0.03142150395672302+0j)</t>
-  </si>
-  <si>
-    <t>(0.1892118244015688+0j)</t>
-  </si>
-  <si>
-    <t>(0.017834531840210787+0j)</t>
-  </si>
-  <si>
-    <t>(-0.03679833231337466+0j)</t>
-  </si>
-  <si>
-    <t>(-0.008750691492449857+0j)</t>
-  </si>
-  <si>
-    <t>(-0.026469148930375257+0j)</t>
-  </si>
-  <si>
-    <t>(0.027312548455567902+0j)</t>
-  </si>
-  <si>
-    <t>(0.07064075543758291+0j)</t>
-  </si>
-  <si>
-    <t>(0.03289021526335843+0j)</t>
-  </si>
-  <si>
-    <t>(0.07188043980308771+0j)</t>
-  </si>
-  <si>
-    <t>(0.0458750845753558+0j)</t>
-  </si>
-  <si>
-    <t>(0.09143870013366452+0j)</t>
-  </si>
-  <si>
-    <t>(0.24716356281796525+0j)</t>
-  </si>
-  <si>
-    <t>(0.038404130951797844+0j)</t>
-  </si>
-  <si>
-    <t>(-0.016328177764011333+0j)</t>
-  </si>
-  <si>
-    <t>(0.01944459286816765+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0032762277142564626+0j)</t>
-  </si>
-  <si>
-    <t>(0.06498830246090243+0j)</t>
-  </si>
-  <si>
-    <t>(0.11973327919580248+0j)</t>
-  </si>
-  <si>
-    <t>(0.07165693186749642+0j)</t>
-  </si>
-  <si>
-    <t>(0.12083690772255781+0j)</t>
-  </si>
-  <si>
-    <t>(0.08782378926671931+0j)</t>
-  </si>
-  <si>
-    <t>(0.14533356573667994+0j)</t>
-  </si>
-  <si>
-    <t>(-9.64607421314313e-06+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05627700063229713+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11389835089808331+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11513477283416199+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11623790020473034+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11720892377222425+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11803170815840235+0j)</t>
-  </si>
-  <si>
-    <t>(-0.1186938359378528+0j)</t>
-  </si>
-  <si>
-    <t>(-0.1192012064136974+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11953839817181058+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11971197719947956+0j)</t>
-  </si>
-  <si>
-    <t>(0.08222228235942868+0j)</t>
-  </si>
-  <si>
-    <t>(-0.022369273527209955+0j)</t>
-  </si>
-  <si>
-    <t>(-0.07781506574735127+0j)</t>
-  </si>
-  <si>
-    <t>(-0.06532354586940213+0j)</t>
-  </si>
-  <si>
-    <t>(-0.07368443095815437+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0490086425435999+0j)</t>
-  </si>
-  <si>
-    <t>(-0.028917835873896198+0j)</t>
-  </si>
-  <si>
-    <t>(-0.04649850363208557+0j)</t>
-  </si>
-  <si>
-    <t>(-0.028271159824374472+0j)</t>
-  </si>
-  <si>
-    <t>(-0.04043878531875962+0j)</t>
-  </si>
-  <si>
-    <t>(-0.019047935988865623+0j)</t>
-  </si>
-  <si>
-    <t>(0.15944000929724447+0j)</t>
-  </si>
-  <si>
-    <t>(0.006983702260421095+0j)</t>
-  </si>
-  <si>
-    <t>(-0.04773280831334567+0j)</t>
-  </si>
-  <si>
-    <t>(-0.023824465410454753+0j)</t>
-  </si>
-  <si>
-    <t>(-0.038964770787876+0j)</t>
-  </si>
-  <si>
-    <t>(0.0070719182518254+0j)</t>
-  </si>
-  <si>
-    <t>(0.04425694843395189+0j)</t>
-  </si>
-  <si>
-    <t>(0.011944811258143466+0j)</t>
-  </si>
-  <si>
-    <t>(0.0454500571976253+0j)</t>
-  </si>
-  <si>
-    <t>(0.023154997506613494+0j)</t>
-  </si>
-  <si>
-    <t>(0.062312716850537485+0j)</t>
-  </si>
-  <si>
-    <t>(0.23290325076173898+0j)</t>
-  </si>
-  <si>
-    <t>(0.033373765247750126+0j)</t>
-  </si>
-  <si>
-    <t>(-0.02131766875743345+0j)</t>
-  </si>
-  <si>
-    <t>(0.012590590592131294+0j)</t>
-  </si>
-  <si>
-    <t>(-0.008891767078526928+0j)</t>
-  </si>
-  <si>
-    <t>(0.05586733721230277+0j)</t>
-  </si>
-  <si>
-    <t>(0.10785711545734719+0j)</t>
-  </si>
-  <si>
-    <t>(0.06230647311289842+0j)</t>
-  </si>
-  <si>
-    <t>(0.10902689065122266+0j)</t>
-  </si>
-  <si>
-    <t>(0.07772351317182154+0j)</t>
-  </si>
-  <si>
-    <t>(0.1323416566623039+0j)</t>
-  </si>
-  <si>
-    <t>(0.3033136822320391+0j)</t>
-  </si>
-  <si>
-    <t>(0.057647841913570544+0j)</t>
-  </si>
-  <si>
-    <t>(0.0025541263697139204+0j)</t>
-  </si>
-  <si>
-    <t>(0.04547242827236726+0j)</t>
-  </si>
-  <si>
-    <t>(0.0179889755344319+0j)</t>
-  </si>
-  <si>
-    <t>(0.09963562205817848+0j)</t>
-  </si>
-  <si>
-    <t>(0.1648591201189965+0j)</t>
-  </si>
-  <si>
-    <t>(0.10714007915029472+0j)</t>
-  </si>
-  <si>
-    <t>(0.16566461643786265+0j)</t>
-  </si>
-  <si>
-    <t>(0.126142962793098+0j)</t>
-  </si>
-  <si>
-    <t>(0.194635799578903+0j)</t>
-  </si>
-  <si>
-    <t>(-5.62448265613283e-06+0j)</t>
-  </si>
-  <si>
-    <t>(-0.056278622572305+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11389968061510845+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11513359134789594+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11623457505869401+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11720313125175853+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11802333374425682+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11868402445878273+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11918906898149478+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11952564373227836+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11969742137220711+0j)</t>
-  </si>
-  <si>
-    <t>(0.09801845547772899+0j)</t>
-  </si>
-  <si>
-    <t>(-0.016209418320756213+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0714166024280976+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05650147508308494+0j)</t>
-  </si>
-  <si>
-    <t>(-0.06624998085055475+0j)</t>
-  </si>
-  <si>
-    <t>(-0.03703832295526407+0j)</t>
-  </si>
-  <si>
-    <t>(-0.013292856287507409+0j)</t>
-  </si>
-  <si>
-    <t>(-0.03395616924237615+0j)</t>
-  </si>
-  <si>
-    <t>(-0.012458857581910357+0j)</t>
-  </si>
-  <si>
-    <t>(-0.026758102340855076+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0015776299468494375+0j)</t>
-  </si>
-  <si>
-    <t>(0.18923073409203858+0j)</t>
-  </si>
-  <si>
-    <t>(0.01784042001882269+0j)</t>
-  </si>
-  <si>
-    <t>(-0.03680062502511079+0j)</t>
-  </si>
-  <si>
-    <t>(-0.008755213049942662+0j)</t>
-  </si>
-  <si>
-    <t>(-0.026482136957247285+0j)</t>
-  </si>
-  <si>
-    <t>(0.027303669605484384+0j)</t>
-  </si>
-  <si>
-    <t>(0.07063550576820393+0j)</t>
-  </si>
-  <si>
-    <t>(0.0328736441185502+0j)</t>
-  </si>
-  <si>
-    <t>(0.07186814869304531+0j)</t>
-  </si>
-  <si>
-    <t>(0.04585515289740891+0j)</t>
-  </si>
-  <si>
-    <t>(0.091426503961692+0j)</t>
-  </si>
-  <si>
-    <t>(0.27551577219584167+0j)</t>
-  </si>
-  <si>
-    <t>(0.04815177155134195+0j)</t>
-  </si>
-  <si>
-    <t>(-0.00674946855890232+0j)</t>
-  </si>
-  <si>
-    <t>(0.03266645560153449+0j)</t>
-  </si>
-  <si>
-    <t>(0.007546277146098175+0j)</t>
-  </si>
-  <si>
-    <t>(0.08262776129205776+0j)</t>
-  </si>
-  <si>
-    <t>(0.14272012469574344+0j)</t>
-  </si>
-  <si>
-    <t>(0.0897569205795941+0j)</t>
-  </si>
-  <si>
-    <t>(0.14370602969753982+0j)</t>
-  </si>
-  <si>
-    <t>(0.1073896729036595+0j)</t>
-  </si>
-  <si>
-    <t>(0.1704971029013781+0j)</t>
-  </si>
-  <si>
-    <t>(0.3578609756844291+0j)</t>
-  </si>
-  <si>
-    <t>(0.07584482942845737+0j)</t>
-  </si>
-  <si>
-    <t>(0.02020689435949053+0j)</t>
-  </si>
-  <si>
-    <t>(0.06979749540712896+0j)</t>
-  </si>
-  <si>
-    <t>(0.03773654166470749+0j)</t>
-  </si>
-  <si>
-    <t>(0.1318921527851422+0j)</t>
-  </si>
-  <si>
-    <t>(0.20685931508652242+0j)</t>
-  </si>
-  <si>
-    <t>(0.14003063526685158+0j)</t>
-  </si>
-  <si>
-    <t>(0.207243018927932+0j)</t>
-  </si>
-  <si>
-    <t>(0.16159945212407198+0j)</t>
-  </si>
-  <si>
-    <t>(0.24033069891786174+0j)</t>
-  </si>
-  <si>
-    <t>(6.10029127956492e-07+0j)</t>
-  </si>
-  <si>
-    <t>(-0.056282625897093756+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11390544412039065+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11513664884764124+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11623483075847602+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11720046313683583+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11801733484038802+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11867557383252754+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11917745378199977+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11951282012792465+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11968229884579827+0j)</t>
-  </si>
-  <si>
-    <t>(0.1136283532816192+0j)</t>
-  </si>
-  <si>
-    <t>(-0.01020702360699787+0j)</t>
-  </si>
-  <si>
-    <t>(-0.06522639173911521+0j)</t>
-  </si>
-  <si>
-    <t>(-0.04796486685651061+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0590837473767951+0j)</t>
-  </si>
-  <si>
-    <t>(-0.02548152284089798+0j)</t>
-  </si>
-  <si>
-    <t>(0.001788435358015717+0j)</t>
-  </si>
-  <si>
-    <t>(-0.021882309571835765+0j)</t>
-  </si>
-  <si>
-    <t>(0.0027665646699338298+0j)</t>
-  </si>
-  <si>
-    <t>(-0.013605623209473568+0j)</t>
-  </si>
-  <si>
-    <t>(0.01523389988417831+0j)</t>
-  </si>
-  <si>
-    <t>(0.21847372215198463+0j)</t>
-  </si>
-  <si>
-    <t>(0.028291556696904214+0j)</t>
-  </si>
-  <si>
-    <t>(-0.026362636245495834+0j)</t>
-  </si>
-  <si>
-    <t>(0.005630609505566808+0j)</t>
-  </si>
-  <si>
-    <t>(-0.014618520590821232+0j)</t>
-  </si>
-  <si>
-    <t>(0.04656124032734456+0j)</t>
-  </si>
-  <si>
-    <t>(0.09573301064199594+0j)</t>
-  </si>
-  <si>
-    <t>(0.05272772449304251+0j)</t>
-  </si>
-  <si>
-    <t>(0.09693477127184014+0j)</t>
-  </si>
-  <si>
-    <t>(0.06735734299188563+0j)</t>
-  </si>
-  <si>
-    <t>(0.11903134052993371+0j)</t>
-  </si>
-  <si>
-    <t>(0.3171557735028934+0j)</t>
-  </si>
-  <si>
-    <t>(0.06228074624243236+0j)</t>
-  </si>
-  <si>
-    <t>(0.007053573712006534+0j)</t>
-  </si>
-  <si>
-    <t>(0.05168192111780091+0j)</t>
-  </si>
-  <si>
-    <t>(0.02303770847762359+0j)</t>
-  </si>
-  <si>
-    <t>(0.10789320075925339+0j)</t>
-  </si>
-  <si>
-    <t>(0.17562382389410164+0j)</t>
-  </si>
-  <si>
-    <t>(0.11558035645018522+0j)</t>
-  </si>
-  <si>
-    <t>(0.17634211117186657+0j)</t>
-  </si>
-  <si>
-    <t>(0.1352550045345244+0j)</t>
-  </si>
-  <si>
-    <t>(0.20638059607437534+0j)</t>
-  </si>
-  <si>
-    <t>(0.410987124454015+0j)</t>
-  </si>
-  <si>
-    <t>(0.09316633367461381+0j)</t>
-  </si>
-  <si>
-    <t>(0.036846492646654135+0j)</t>
-  </si>
-  <si>
-    <t>(0.09272051411752459+0j)</t>
-  </si>
-  <si>
-    <t>(0.05624350266282505+0j)</t>
-  </si>
-  <si>
-    <t>(0.16219174032731268+0j)</t>
-  </si>
-  <si>
-    <t>(0.246304640857501+0j)</t>
-  </si>
-  <si>
-    <t>(0.17081218381993182+0j)</t>
-  </si>
-  <si>
-    <t>(0.24617895895273822+0j)</t>
-  </si>
-  <si>
-    <t>(0.1947341319368432+0j)</t>
-  </si>
-  <si>
-    <t>(0.28309657875650834+0j)</t>
-  </si>
-  <si>
-    <t>(8.638046478019225e-06+0j)</t>
-  </si>
-  <si>
-    <t>(-0.056288631282698134+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11391540540300704+0j)</t>
-  </si>
-  <si>
-    <t>(-0.1151440297483036+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11623918574955401+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11720200296607788+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11801554362916632+0j)</t>
-  </si>
-  <si>
-    <t>(-0.1186706536534989+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11916929224561472+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11950296522235251+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11967030868235154+0j)</t>
-  </si>
-  <si>
-    <t>(0.12905830142994726+0j)</t>
-  </si>
-  <si>
-    <t>(-0.004348585163414464+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05922444196027483+0j)</t>
-  </si>
-  <si>
-    <t>(-0.03968660771799902+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0521592689192635+0j)</t>
-  </si>
-  <si>
-    <t>(-0.014298188188148426+0j)</t>
-  </si>
-  <si>
-    <t>(0.016378800762674638+0j)</t>
-  </si>
-  <si>
-    <t>(-0.010230327502433688+0j)</t>
-  </si>
-  <si>
-    <t>(0.017463367394841497+0j)</t>
-  </si>
-  <si>
-    <t>(-0.000928229287426047+0j)</t>
-  </si>
-  <si>
-    <t>(0.03145241439701184+0j)</t>
-  </si>
-  <si>
-    <t>(0.24720795582302316+0j)</t>
-  </si>
-  <si>
-    <t>(0.038383924066133494+0j)</t>
-  </si>
-  <si>
-    <t>(-0.01635557199535554+0j)</t>
-  </si>
-  <si>
-    <t>(0.019420825874920628+0j)</t>
-  </si>
-  <si>
-    <t>(-0.0032903950313702803+0j)</t>
-  </si>
-  <si>
-    <t>(0.06497370373159059+0j)</t>
-  </si>
-  <si>
-    <t>(0.11971949590219279+0j)</t>
-  </si>
-  <si>
-    <t>(0.07165446497652884+0j)</t>
-  </si>
-  <si>
-    <t>(0.12083445015600056+0j)</t>
-  </si>
-  <si>
-    <t>(0.08782823398311072+0j)</t>
-  </si>
-  <si>
-    <t>(0.1453345144163548+0j)</t>
-  </si>
-  <si>
-    <t>(0.357909463594377+0j)</t>
-  </si>
-  <si>
-    <t>(0.07584669476643999+0j)</t>
-  </si>
-  <si>
-    <t>(0.02020237326708487+0j)</t>
-  </si>
-  <si>
-    <t>(0.06979136167266642+0j)</t>
-  </si>
-  <si>
-    <t>(0.03772640819714109+0j)</t>
-  </si>
-  <si>
-    <t>(0.13188785308546674+0j)</t>
-  </si>
-  <si>
-    <t>(0.20686310707047623+0j)</t>
-  </si>
-  <si>
-    <t>(0.1400287959515625+0j)</t>
-  </si>
-  <si>
-    <t>(0.2072508537193756+0j)</t>
-  </si>
-  <si>
-    <t>(0.16160238360103069+0j)</t>
-  </si>
-  <si>
-    <t>(0.24034551853915276+0j)</t>
-  </si>
-  <si>
-    <t>(0.4628362136438125+0j)</t>
-  </si>
-  <si>
-    <t>(0.10974015055646848+0j)</t>
-  </si>
-  <si>
-    <t>(0.05263163077110521+0j)</t>
-  </si>
-  <si>
-    <t>(0.11446221063048494+0j)</t>
-  </si>
-  <si>
-    <t>(0.07371160300358755+0j)</t>
-  </si>
-  <si>
-    <t>(0.19085104460117885+0j)</t>
-  </si>
-  <si>
-    <t>(0.28361116533639824+0j)</t>
-  </si>
-  <si>
-    <t>(0.19983526550381533+0j)</t>
-  </si>
-  <si>
-    <t>(0.28291222649897513+0j)</t>
-  </si>
-  <si>
-    <t>(0.22593775385256765+0j)</t>
-  </si>
-  <si>
-    <t>(0.3234241430647014+0j)</t>
-  </si>
-  <si>
-    <t>(1.8149637071169624e-05+0j)</t>
-  </si>
-  <si>
-    <t>(-0.056296267665422235+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11392918435679683+0j)</t>
-  </si>
-  <si>
-    <t>(-0.1151556187018106+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11624785355118883+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11720845404540516+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11801929378683133+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11867083973386214+0j)</t>
-  </si>
-  <si>
-    <t>(-0.1191667980001185+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11949835954704816+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11966429141001715+0j)</t>
-  </si>
-  <si>
-    <t>(0.14431438451922354+0j)</t>
-  </si>
-  <si>
-    <t>(0.0013773879440492833+0j)</t>
-  </si>
-  <si>
-    <t>(-0.05339356436107544+0j)</t>
-  </si>
-  <si>
-    <t>(-0.03164362710695245+0j)</t>
-  </si>
-  <si>
-    <t>(-0.045454006722450584+0j)</t>
-  </si>
-  <si>
-    <t>(-0.003454422597212593+0j)</t>
-  </si>
-  <si>
-    <t>(0.03052283174627509+0j)</t>
-  </si>
-  <si>
-    <t>(0.001039247336974582+0j)</t>
-  </si>
-  <si>
-    <t>(0.03168088265624985+0j)</t>
-  </si>
-  <si>
-    <t>(0.011319108448023663+0j)</t>
-  </si>
-  <si>
-    <t>(0.04713363595530335+0j)</t>
-  </si>
-  <si>
-    <t>(0.27546676481144644+0j)</t>
-  </si>
-  <si>
-    <t>(0.04815553968417356+0j)</t>
-  </si>
-  <si>
-    <t>(-0.006728697950942046+0j)</t>
-  </si>
-  <si>
-    <t>(0.03268566936970085+0j)</t>
-  </si>
-  <si>
-    <t>(0.007568550226130962+0j)</t>
-  </si>
-  <si>
-    <t>(0.0826437080757524+0j)</t>
-  </si>
-  <si>
-    <t>(0.1427301353997771+0j)</t>
-  </si>
-  <si>
-    <t>(0.08977047911003677+0j)</t>
-  </si>
-  <si>
-    <t>(0.1437132683900883+0j)</t>
-  </si>
-  <si>
-    <t>(0.10739938891504379+0j)</t>
-  </si>
-  <si>
-    <t>(0.17049999387885087+0j)</t>
-  </si>
-  <si>
-    <t>(0.39784843463119224+0j)</t>
-  </si>
-  <si>
-    <t>(0.08891742863684006+0j)</t>
-  </si>
-  <si>
-    <t>(0.03278305761164984+0j)</t>
-  </si>
-  <si>
-    <t>(0.08711460566491992+0j)</t>
-  </si>
-  <si>
-    <t>(0.051723225549796956+0j)</t>
-  </si>
-  <si>
-    <t>(0.15478485296257652+0j)</t>
-  </si>
-  <si>
-    <t>(0.23666553694926268+0j)</t>
-  </si>
-  <si>
-    <t>(0.1632956903774638+0j)</t>
-  </si>
-  <si>
-    <t>(0.23667467515936924+0j)</t>
-  </si>
-  <si>
-    <t>(0.18664835606724703+0j)</t>
-  </si>
-  <si>
-    <t>(0.27266284682077874+0j)</t>
-  </si>
-  <si>
-    <t>(0.5135255893679577+0j)</t>
-  </si>
-  <si>
-    <t>(0.1256648257567948+0j)</t>
-  </si>
-  <si>
-    <t>(0.06768294819390866+0j)</t>
-  </si>
-  <si>
-    <t>(0.13519037803330802+0j)</t>
-  </si>
-  <si>
-    <t>(0.09029318218794163+0j)</t>
-  </si>
-  <si>
-    <t>(0.21810955569363508+0j)</t>
-  </si>
-  <si>
-    <t>(0.3190931694668505+0j)</t>
-  </si>
-  <si>
-    <t>(0.22736342879204827+0j)</t>
-  </si>
-  <si>
-    <t>(0.3177733760347133+0j)</t>
-  </si>
-  <si>
-    <t>(0.25550324492942256+0j)</t>
-  </si>
-  <si>
-    <t>(0.3616816394892024+0j)</t>
-  </si>
-  <si>
-    <t>(2.8927960502851472e-05+0j)</t>
-  </si>
-  <si>
-    <t>(-0.056305218500470454+0j)</t>
-  </si>
-  <si>
-    <t>(-0.1139463728734692+0j)</t>
-  </si>
-  <si>
-    <t>(-0.1151712167093135+0j)</t>
-  </si>
-  <si>
-    <t>(-0.1162608679180659+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11722025555506356+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11802953236709336+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11867723707755022+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11917158839107897+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11950065373363787+0j)</t>
-  </si>
-  <si>
-    <t>(-0.11966635486364834+0j)</t>
-  </si>
-  <si>
-    <t>(0.15940251017277565+0j)</t>
-  </si>
-  <si>
-    <t>(0.006980812646089126+0j)</t>
-  </si>
-  <si>
-    <t>(-0.04771892268957646+0j)</t>
-  </si>
-  <si>
-    <t>(-0.023816107222183008+0j)</t>
-  </si>
-  <si>
-    <t>(-0.03894862103020876+0j)</t>
-  </si>
-  <si>
-    <t>(0.0070787872672185845+0j)</t>
-  </si>
-  <si>
-    <t>(0.0442586692367478+0j)</t>
-  </si>
-  <si>
-    <t>(0.011960179138269432+0j)</t>
-  </si>
-  <si>
-    <t>(0.04546130808179909+0j)</t>
-  </si>
-  <si>
-    <t>(0.023174908337527982+0j)</t>
-  </si>
-  <si>
-    <t>(0.06232523613777708+0j)</t>
-  </si>
-  <si>
-    <t>(0.30327913974743775+0j)</t>
-  </si>
-  <si>
-    <t>(0.05763783387036946+0j)</t>
-  </si>
-  <si>
-    <t>(0.0025594331605961443+0j)</t>
-  </si>
-  <si>
-    <t>(0.04548240092470059+0j)</t>
-  </si>
-  <si>
-    <t>(0.0180120231841103+0j)</t>
-  </si>
-  <si>
-    <t>(0.09965452697989377+0j)</t>
-  </si>
-  <si>
-    <t>(0.16487454203135313+0j)</t>
-  </si>
-  <si>
-    <t>(0.10716990723351383+0j)</t>
-  </si>
-  <si>
-    <t>(0.16568922297672992+0j)</t>
-  </si>
-  <si>
-    <t>(0.12617679988159752+0j)</t>
-  </si>
-  <si>
-    <t>(0.19466011062664706+0j)</t>
-  </si>
-  <si>
-    <t>(0.43703328914986883+0j)</t>
-  </si>
-  <si>
-    <t>(0.10154763907534259+0j)</t>
-  </si>
-  <si>
-    <t>(0.04486416883414648+0j)</t>
-  </si>
-  <si>
-    <t>(0.10374695777026696+0j)</t>
-  </si>
-  <si>
-    <t>(0.06511573532491127+0j)</t>
-  </si>
-  <si>
-    <t>(0.17672124411375514+0j)</t>
-  </si>
-  <si>
-    <t>(0.265211105779141+0j)</t>
-  </si>
-  <si>
-    <t>(0.18553333714008705+0j)</t>
-  </si>
-  <si>
-    <t>(0.26480445927397994+0j)</t>
-  </si>
-  <si>
-    <t>(0.21056297699619225+0j)</t>
-  </si>
-  <si>
-    <t>(0.3035456936493369+0j)</t>
-  </si>
-  <si>
-    <t>(0.5631528522089848+0j)</t>
-  </si>
-  <si>
-    <t>(0.14101835702711862+0j)</t>
-  </si>
-  <si>
-    <t>(0.08209477178059944+0j)</t>
-  </si>
-  <si>
-    <t>(0.1550361746176363+0j)</t>
-  </si>
-  <si>
-    <t>(0.10610663085351739+0j)</t>
-  </si>
-  <si>
-    <t>(0.24415359761291733+0j)</t>
-  </si>
-  <si>
-    <t>(0.3529948755546369+0j)</t>
-  </si>
-  <si>
-    <t>(0.253600659526805+0j)</t>
-  </si>
-  <si>
-    <t>(0.3510181755444845+0j)</t>
-  </si>
-  <si>
-    <t>(0.2836567548941969+0j)</t>
-  </si>
-  <si>
-    <t>(0.3981536121273402+0j)</t>
+    <t>(-0.10107672284163818+0.0011892718926374325j)</t>
+  </si>
+  <si>
+    <t>(-0.10106050588092554-0.0009200398332796695j)</t>
+  </si>
+  <si>
+    <t>(-0.10245663177043864+0.0020631927923490043j)</t>
+  </si>
+  <si>
+    <t>(-0.1037655985604767+0.004846583311394344j)</t>
+  </si>
+  <si>
+    <t>(-0.10474610513181504+0.006686927835102954j)</t>
+  </si>
+  <si>
+    <t>(-0.10537126148352388+0.007611300941655866j)</t>
+  </si>
+  <si>
+    <t>(-0.10524631589133368+0.006773064652520169j)</t>
+  </si>
+  <si>
+    <t>(-0.10589792893461171+0.008015074525492365j)</t>
+  </si>
+  <si>
+    <t>(-0.10570293252964404+0.007395552461778363j)</t>
+  </si>
+  <si>
+    <t>(-0.10588950528167874+0.007718769733541606j)</t>
+  </si>
+  <si>
+    <t>(-0.10591804035905082+0.007748552811192123j)</t>
+  </si>
+  <si>
+    <t>(-0.10197389080838737+0.0003536537062722754j)</t>
+  </si>
+  <si>
+    <t>(-0.10195186224990425+0.0012669262861895497j)</t>
+  </si>
+  <si>
+    <t>(-0.10320489959066034+0.002772432764935484j)</t>
+  </si>
+  <si>
+    <t>(-0.10449651097134845+0.00399948713231736j)</t>
+  </si>
+  <si>
+    <t>(-0.10549810876602145+0.004970458063543289j)</t>
+  </si>
+  <si>
+    <t>(-0.10611777760489699+0.005806410609903435j)</t>
+  </si>
+  <si>
+    <t>(-0.10584306409147831+0.006848417501097786j)</t>
+  </si>
+  <si>
+    <t>(-0.10654087109528787+0.007356613775596144j)</t>
+  </si>
+  <si>
+    <t>(-0.10624234394265952+0.00826477214363793j)</t>
+  </si>
+  <si>
+    <t>(-0.10643490331888646+0.008658807178472777j)</t>
+  </si>
+  <si>
+    <t>(-0.10645830249948131+0.008922253064700616j)</t>
+  </si>
+  <si>
+    <t>(-0.10218318330629042+0.00023676675184075802j)</t>
+  </si>
+  <si>
+    <t>(-0.10224532307852426+0.002270892383833945j)</t>
+  </si>
+  <si>
+    <t>(-0.10351832572530645+0.003230549207919955j)</t>
+  </si>
+  <si>
+    <t>(-0.10481431766575418+0.0038754964765595006j)</t>
+  </si>
+  <si>
+    <t>(-0.1058247461794221+0.004516886695276297j)</t>
+  </si>
+  <si>
+    <t>(-0.1064699628167045+0.005307674875979574j)</t>
+  </si>
+  <si>
+    <t>(-0.10632526216253736+0.006995236126193304j)</t>
+  </si>
+  <si>
+    <t>(-0.10700875360900605+0.007218491046436356j)</t>
+  </si>
+  <si>
+    <t>(-0.10684985533869439+0.008610399675203075j)</t>
+  </si>
+  <si>
+    <t>(-0.10707315226494547+0.008997069178624487j)</t>
+  </si>
+  <si>
+    <t>(-0.10713009591341115+0.009319099955930513j)</t>
+  </si>
+  <si>
+    <t>(-0.10213832482167555+0.000768452722438281j)</t>
+  </si>
+  <si>
+    <t>(-0.10218002179606238+0.0028365213380115942j)</t>
+  </si>
+  <si>
+    <t>(-0.10361186316474284+0.0037350350366546175j)</t>
+  </si>
+  <si>
+    <t>(-0.10499454731661212+0.004330165524481991j)</t>
+  </si>
+  <si>
+    <t>(-0.10605622115735597+0.004938081133625154j)</t>
+  </si>
+  <si>
+    <t>(-0.10674570497706161+0.0056929707968952255j)</t>
+  </si>
+  <si>
+    <t>(-0.10667884824924334+0.007263750049922122j)</t>
+  </si>
+  <si>
+    <t>(-0.10737169667142228+0.0074565779601177195j)</t>
+  </si>
+  <si>
+    <t>(-0.10725234528689039+0.008678880208890863j)</t>
+  </si>
+  <si>
+    <t>(-0.10747786039847064+0.008999500225193427j)</t>
+  </si>
+  <si>
+    <t>(-0.10753553544581122+0.009267257745247975j)</t>
+  </si>
+  <si>
+    <t>(-0.10206166126757454+0.0017990461590579932j)</t>
+  </si>
+  <si>
+    <t>(-0.10201228788453573+0.00325556040990981j)</t>
+  </si>
+  <si>
+    <t>(-0.10365529343986894+0.004362754153397432j)</t>
+  </si>
+  <si>
+    <t>(-0.10516391100106273+0.005212112854635823j)</t>
+  </si>
+  <si>
+    <t>(-0.10630472875541795+0.005952926605936606j)</t>
+  </si>
+  <si>
+    <t>(-0.10704361878007065+0.006668569605685933j)</t>
+  </si>
+  <si>
+    <t>(-0.1069190484308326+0.007667568161035113j)</t>
+  </si>
+  <si>
+    <t>(-0.10765242306258156+0.007972853342925914j)</t>
+  </si>
+  <si>
+    <t>(-0.10737538392316427+0.008645944559645943j)</t>
+  </si>
+  <si>
+    <t>(-0.10755353872375814+0.008866569957623869j)</t>
+  </si>
+  <si>
+    <t>(-0.10755663774151047+0.009016165612058483j)</t>
+  </si>
+  <si>
+    <t>(-0.10114073470256023+0.0011685009317761459j)</t>
+  </si>
+  <si>
+    <t>(-0.10223761495251152+0.0009298890532907531j)</t>
+  </si>
+  <si>
+    <t>(-0.10297419632264018+0.002819553345460143j)</t>
+  </si>
+  <si>
+    <t>(-0.10361800546859852+0.0045696109942899065j)</t>
+  </si>
+  <si>
+    <t>(-0.10421106835506193+0.00586362237974029j)</t>
+  </si>
+  <si>
+    <t>(-0.10474661879416505+0.00670767157037783j)</t>
+  </si>
+  <si>
+    <t>(-0.10522282819405318+0.006715237354296764j)</t>
+  </si>
+  <si>
+    <t>(-0.1055566797387107+0.007563142846824389j)</t>
+  </si>
+  <si>
+    <t>(-0.10580493133957503+0.007502785418818486j)</t>
+  </si>
+  <si>
+    <t>(-0.10596299247081951+0.007792274918578649j)</t>
+  </si>
+  <si>
+    <t>(-0.10603756066948122+0.007875285011706002j)</t>
+  </si>
+  <si>
+    <t>(-0.09703180222863192+0.0008763317834225926j)</t>
+  </si>
+  <si>
+    <t>(-0.08837095985787148+0.0019660004435110845j)</t>
+  </si>
+  <si>
+    <t>(-0.09265335234573087+0.0028477559880119825j)</t>
+  </si>
+  <si>
+    <t>(-0.09845011676006181+0.003699984485337437j)</t>
+  </si>
+  <si>
+    <t>(-0.10249783329019556+0.0045050230863560485j)</t>
+  </si>
+  <si>
+    <t>(-0.10359326699075447+0.005196996790628889j)</t>
+  </si>
+  <si>
+    <t>(-0.09511207309628511+0.005579530379552952j)</t>
+  </si>
+  <si>
+    <t>(-0.09900448598187739+0.006095034557037831j)</t>
+  </si>
+  <si>
+    <t>(-0.0910540315594727+0.006188281610562693j)</t>
+  </si>
+  <si>
+    <t>(-0.09065616824271436+0.006370727990468765j)</t>
+  </si>
+  <si>
+    <t>(-0.08934843761742209+0.006425279650506341j)</t>
+  </si>
+  <si>
+    <t>(-0.09277308047292272+0.0007155418530697558j)</t>
+  </si>
+  <si>
+    <t>(-0.07446733868660405+0.0019224295968475699j)</t>
+  </si>
+  <si>
+    <t>(-0.08231583928012724+0.002451349017888409j)</t>
+  </si>
+  <si>
+    <t>(-0.0932286036964369+0.0030750322570279476j)</t>
+  </si>
+  <si>
+    <t>(-0.10069707791261479+0.003766657711834372j)</t>
+  </si>
+  <si>
+    <t>(-0.10235755593135218+0.004367745869144622j)</t>
+  </si>
+  <si>
+    <t>(-0.08508466186796292+0.004465544799475831j)</t>
+  </si>
+  <si>
+    <t>(-0.09248950285721366+0.004950648263494375j)</t>
+  </si>
+  <si>
+    <t>(-0.07649151856788551+0.004710430642796265j)</t>
+  </si>
+  <si>
+    <t>(-0.07555398310154392+0.004796735944828555j)</t>
+  </si>
+  <si>
+    <t>(-0.0728903609797943+0.00476522838236607j)</t>
+  </si>
+  <si>
+    <t>(-0.08847938461623767+0.0006952777327552251j)</t>
+  </si>
+  <si>
+    <t>(-0.060506709389476866+0.0013906575013852753j)</t>
+  </si>
+  <si>
+    <t>(-0.07198024382365771+0.0019235255720625789j)</t>
+  </si>
+  <si>
+    <t>(-0.08803339307407683+0.0026669955879020306j)</t>
+  </si>
+  <si>
+    <t>(-0.09892809650480475+0.003433429749850608j)</t>
+  </si>
+  <si>
+    <t>(-0.10115923865153695+0.003972858871228649j)</t>
+  </si>
+  <si>
+    <t>(-0.07513564317591123+0.0034901289229062058j)</t>
+  </si>
+  <si>
+    <t>(-0.08604667164095538+0.004085690712459653j)</t>
+  </si>
+  <si>
+    <t>(-0.06204098859100221+0.003318949998622885j)</t>
+  </si>
+  <si>
+    <t>(-0.06056927649165439+0.0033246489794916375j)</t>
+  </si>
+  <si>
+    <t>(-0.056556707209724895+0.0031909937584258933j)</t>
+  </si>
+  <si>
+    <t>(-0.08421112984715282+0.0007887281798058614j)</t>
+  </si>
+  <si>
+    <t>(-0.04658471047714573+0.0006609177111118217j)</t>
+  </si>
+  <si>
+    <t>(-0.06171216112083253+0.0013943600525481083j)</t>
+  </si>
+  <si>
+    <t>(-0.0829048417564534+0.0024331982252775884j)</t>
+  </si>
+  <si>
+    <t>(-0.09721712259573624+0.0033622463941463785j)</t>
+  </si>
+  <si>
+    <t>(-0.10001907072249758+0.0038533488244873815j)</t>
+  </si>
+  <si>
+    <t>(-0.06529654932706537+0.0026936439758456394j)</t>
+  </si>
+  <si>
+    <t>(-0.07969665042697778+0.0034544762813868268j)</t>
+  </si>
+  <si>
+    <t>(-0.04773087081498537+0.0021289265527390504j)</t>
+  </si>
+  <si>
+    <t>(-0.04572815451305268+0.0020728854509134594j)</t>
+  </si>
+  <si>
+    <t>(-0.04037397493860338+0.001843893388899948j)</t>
+  </si>
+  <si>
+    <t>(-0.10118718793325353+0.0011274855727848282j)</t>
+  </si>
+  <si>
+    <t>(-0.10295675190822162+0.002040768391085281j)</t>
+  </si>
+  <si>
+    <t>(-0.10328560914764522+0.0032757242070924563j)</t>
+  </si>
+  <si>
+    <t>(-0.10353240925389445+0.004396016965430549j)</t>
+  </si>
+  <si>
+    <t>(-0.10390148047187585+0.005353263565439226j)</t>
+  </si>
+  <si>
+    <t>(-0.10438946974175375+0.006149854006032253j)</t>
+  </si>
+  <si>
+    <t>(-0.10520885129858366+0.00672011786268202j)</t>
+  </si>
+  <si>
+    <t>(-0.10536599586532455+0.007316145623848048j)</t>
+  </si>
+  <si>
+    <t>(-0.10586306762785874+0.0076541907864650285j)</t>
+  </si>
+  <si>
+    <t>(-0.10600667696216332+0.00793413761991363j)</t>
+  </si>
+  <si>
+    <t>(-0.10610763753140891+0.008063287024340239j)</t>
+  </si>
+  <si>
+    <t>(-0.09233160513748487+0.0012065445446690208j)</t>
+  </si>
+  <si>
+    <t>(-0.07481876260571768+0.0022109966300037673j)</t>
+  </si>
+  <si>
+    <t>(-0.08224347779497072+0.002704050179896114j)</t>
+  </si>
+  <si>
+    <t>(-0.09266162891534112+0.003363901785492439j)</t>
+  </si>
+  <si>
+    <t>(-0.09981732409569409+0.004087998568460517j)</t>
+  </si>
+  <si>
+    <t>(-0.10139669192878886+0.004665848281802145j)</t>
+  </si>
+  <si>
+    <t>(-0.08462617667789189+0.004452466212397982j)</t>
+  </si>
+  <si>
+    <t>(-0.09175968124813379+0.005008683307586586j)</t>
+  </si>
+  <si>
+    <t>(-0.07613269721912518+0.00444519063287877j)</t>
+  </si>
+  <si>
+    <t>(-0.07516438127027718+0.004478731654373651j)</t>
+  </si>
+  <si>
+    <t>(-0.07253446784337071+0.004378509804248525j)</t>
+  </si>
+  <si>
+    <t>(-0.08367219810061904+0.0010042250971965556j)</t>
+  </si>
+  <si>
+    <t>(-0.04696858096388328+0.0015418452840975367j)</t>
+  </si>
+  <si>
+    <t>(-0.06149073829222529+0.0018065409318546554j)</t>
+  </si>
+  <si>
+    <t>(-0.08203663321868385+0.0024011078014870976j)</t>
+  </si>
+  <si>
+    <t>(-0.09593141462234224+0.0030800944726220364j)</t>
+  </si>
+  <si>
+    <t>(-0.09859394074445849+0.0035099498261907357j)</t>
+  </si>
+  <si>
+    <t>(-0.06445816586830896+0.0026394580748185037j)</t>
+  </si>
+  <si>
+    <t>(-0.07850495364020066+0.003236585844445329j)</t>
+  </si>
+  <si>
+    <t>(-0.04703336339485652+0.0020861013106965053j)</t>
+  </si>
+  <si>
+    <t>(-0.04500757702655029+0.0020030469717195543j)</t>
+  </si>
+  <si>
+    <t>(-0.03971455457189897+0.0017823679019542754j)</t>
+  </si>
+  <si>
+    <t>(-0.07511574392686841+0.0006106792908123234j)</t>
+  </si>
+  <si>
+    <t>(-0.019274534216901396+0.000525137314330241j)</t>
+  </si>
+  <si>
+    <t>(-0.04096008966465329+0.0008312480223375949j)</t>
+  </si>
+  <si>
+    <t>(-0.07162463654784545+0.0015161521529651694j)</t>
+  </si>
+  <si>
+    <t>(-0.09222189485852492+0.0022050360691308825j)</t>
+  </si>
+  <si>
+    <t>(-0.09596653405940966+0.0025259896595779437j)</t>
+  </si>
+  <si>
+    <t>(-0.04475089019597976+0.00127259799147618j)</t>
+  </si>
+  <si>
+    <t>(-0.06563904384474328+0.0018912034811476863j)</t>
+  </si>
+  <si>
+    <t>(-0.018680921612614965+0.0005285881020654137j)</t>
+  </si>
+  <si>
+    <t>(-0.015668830878265795+0.00042433641033434597j)</t>
+  </si>
+  <si>
+    <t>(-0.00779941398416842+0.00018172438904685842j)</t>
+  </si>
+  <si>
+    <t>(-0.06662474406730524+9.374024402548608e-05j)</t>
+  </si>
+  <si>
+    <t>(0.008233018274198705-0.00056881350791168j)</t>
+  </si>
+  <si>
+    <t>(-0.020667947796996874-9.576315125281771e-05j)</t>
+  </si>
+  <si>
+    <t>(-0.06141042073145768+0.0007079573596525607j)</t>
+  </si>
+  <si>
+    <t>(-0.08865126664157515+0.0013958262054281035j)</t>
+  </si>
+  <si>
+    <t>(-0.09347532017916518+0.0016287661137906677j)</t>
+  </si>
+  <si>
+    <t>(-0.025537180844267+0.000297235543460435j)</t>
+  </si>
+  <si>
+    <t>(-0.053167718895741775+0.0008767518918409959j)</t>
+  </si>
+  <si>
+    <t>(0.008855936922001139-0.00034598036116338757j)</t>
+  </si>
+  <si>
+    <t>(0.01278004268387955-0.0004037624576099614j)</t>
+  </si>
+  <si>
+    <t>(0.02312951665345682-0.0005875127605846143j)</t>
+  </si>
+  <si>
+    <t>(-0.10120682217703633+0.0010955518235743586j)</t>
+  </si>
+  <si>
+    <t>(-0.10331238098621696+0.002682127209529935j)</t>
+  </si>
+  <si>
+    <t>(-0.10343882721309137+0.00354555929388117j)</t>
+  </si>
+  <si>
+    <t>(-0.10349339125096899+0.0042988523869482665j)</t>
+  </si>
+  <si>
+    <t>(-0.10375763115616828+0.005055357222798195j)</t>
+  </si>
+  <si>
+    <t>(-0.10422767789181496+0.005822564416393956j)</t>
+  </si>
+  <si>
+    <t>(-0.10522121700475619+0.006750330006340259j)</t>
+  </si>
+  <si>
+    <t>(-0.10529735419432976+0.007188516182514363j)</t>
+  </si>
+  <si>
+    <t>(-0.10592538552457348+0.00779523240292096j)</t>
+  </si>
+  <si>
+    <t>(-0.10606757409338584+0.008074741035832281j)</t>
+  </si>
+  <si>
+    <t>(-0.10618538323238733+0.008238746647009059j)</t>
+  </si>
+  <si>
+    <t>(-0.08781610555377022+0.0013648935421708502j)</t>
+  </si>
+  <si>
+    <t>(-0.06124381805877052+0.0021174919151714148j)</t>
+  </si>
+  <si>
+    <t>(-0.07192913475358921+0.002399508232030432j)</t>
+  </si>
+  <si>
+    <t>(-0.08708494643084555+0.002992506939756695j)</t>
+  </si>
+  <si>
+    <t>(-0.09740942661543603+0.0036890449127962065j)</t>
+  </si>
+  <si>
+    <t>(-0.09948231669056143+0.0041751645178933j)</t>
+  </si>
+  <si>
+    <t>(-0.07435650556047772+0.003463740933351659j)</t>
+  </si>
+  <si>
+    <t>(-0.08477398452593973+0.004070454654428746j)</t>
+  </si>
+  <si>
+    <t>(-0.061463149928900666+0.003021070936202937j)</t>
+  </si>
+  <si>
+    <t>(-0.05994705796725914+0.0029597214405697983j)</t>
+  </si>
+  <si>
+    <t>(-0.05600742648109592+0.0027558415253145343j)</t>
+  </si>
+  <si>
+    <t>(-0.07481800034535324+0.0011195847135354448j)</t>
+  </si>
+  <si>
+    <t>(-0.01968949018217124+0.0011394761675116159j)</t>
+  </si>
+  <si>
+    <t>(-0.040990879370296475+0.0012711555581564956j)</t>
+  </si>
+  <si>
+    <t>(-0.07119232097094341+0.0018220331465008625j)</t>
+  </si>
+  <si>
+    <t>(-0.09148706929619503+0.002432713541326583j)</t>
+  </si>
+  <si>
+    <t>(-0.09514373019134162+0.0027077871060346226j)</t>
+  </si>
+  <si>
+    <t>(-0.04441346236499441+0.0013927806051795345j)</t>
+  </si>
+  <si>
+    <t>(-0.06502761032143557+0.001974935013593648j)</t>
+  </si>
+  <si>
+    <t>(-0.01844654448555407+0.0005142354009453952j)</t>
+  </si>
+  <si>
+    <t>(-0.015405886101146102+0.00036870056625884116j)</t>
+  </si>
+  <si>
+    <t>(-0.007574088805078159+9.402165229540542e-05j)</t>
+  </si>
+  <si>
+    <t>(-0.06200779255264545+0.0005169010148523887j)</t>
+  </si>
+  <si>
+    <t>(0.021483992514500734+0.00013924222461331106j)</t>
+  </si>
+  <si>
+    <t>(-0.010546853383061177+0.00030822720920540544j)</t>
+  </si>
+  <si>
+    <t>(-0.05573093800178712+0.0007632763438411511j)</t>
+  </si>
+  <si>
+    <t>(-0.08588623460886402+0.0011907136929069724j)</t>
+  </si>
+  <si>
+    <t>(-0.09111801449000057+0.001294407533551147j)</t>
+  </si>
+  <si>
+    <t>(-0.015490289052178741+0.00025558050914945625j)</t>
+  </si>
+  <si>
+    <t>(-0.04610813666804588+0.0006077026540398452j)</t>
+  </si>
+  <si>
+    <t>(0.022878409441638502-0.00029472318643672336j)</t>
+  </si>
+  <si>
+    <t>(0.027282294854914305-0.0003557916784335619j)</t>
+  </si>
+  <si>
+    <t>(0.03880212724644193-0.000487749580861899j)</t>
+  </si>
+  <si>
+    <t>(-0.04930235350920333-0.00031370452460538126j)</t>
+  </si>
+  <si>
+    <t>(0.06225130001287185-0.0006720853377928133j)</t>
+  </si>
+  <si>
+    <t>(0.019404943277092735-0.0004237439701201801j)</t>
+  </si>
+  <si>
+    <t>(-0.04065024215885002-0.00019819092361179251j)</t>
+  </si>
+  <si>
+    <t>(-0.08052639029962363-7.487803659721778e-05j)</t>
+  </si>
+  <si>
+    <t>(-0.08732479563523605-0.00012143883664344232j)</t>
+  </si>
+  <si>
+    <t>(0.012409400101593731-0.00018462118946306513j)</t>
+  </si>
+  <si>
+    <t>(-0.02798668597784026-0.0002484778516063991j)</t>
+  </si>
+  <si>
+    <t>(0.062484339714716786+0.0001263679958283787j)</t>
+  </si>
+  <si>
+    <t>(0.06809378745515035+0.00025567646642379394j)</t>
+  </si>
+  <si>
+    <t>(0.08309338113834781+0.00041366233860821587j)</t>
+  </si>
+  <si>
+    <t>(-0.10120105229009295+0.0010934095444724659j)</t>
+  </si>
+  <si>
+    <t>(-0.1034021774636233+0.0030203126144848313j)</t>
+  </si>
+  <si>
+    <t>(-0.10347965807300016+0.003698857321897849j)</t>
+  </si>
+  <si>
+    <t>(-0.10348785965004023+0.00426325661631386j)</t>
+  </si>
+  <si>
+    <t>(-0.10372911735982708+0.004912301269410197j)</t>
+  </si>
+  <si>
+    <t>(-0.1042008034460466+0.005660268485977776j)</t>
+  </si>
+  <si>
+    <t>(-0.10526040495833008+0.006781980012205467j)</t>
+  </si>
+  <si>
+    <t>(-0.10531749598834275+0.007130301859279445j)</t>
+  </si>
+  <si>
+    <t>(-0.1060045353070788+0.007889017334311306j)</t>
+  </si>
+  <si>
+    <t>(-0.1061544661963261+0.008168100866729642j)</t>
+  </si>
+  <si>
+    <t>(-0.1062838920105911+0.008352334101446887j)</t>
+  </si>
+  <si>
+    <t>(-0.08344496242516256+0.0013724966065340586j)</t>
+  </si>
+  <si>
+    <t>(-0.047624474270888326+0.0017740895641008153j)</t>
+  </si>
+  <si>
+    <t>(-0.06168504117981893+0.0019795087329717736j)</t>
+  </si>
+  <si>
+    <t>(-0.08168652924954657+0.0025899928217539944j)</t>
+  </si>
+  <si>
+    <t>(-0.09523492577340406+0.0032900219928543124j)</t>
+  </si>
+  <si>
+    <t>(-0.09781093850739014+0.003701245757033507j)</t>
+  </si>
+  <si>
+    <t>(-0.0642840668103739+0.002608948383671836j)</t>
+  </si>
+  <si>
+    <t>(-0.0780215987246767+0.0032602685137194183j)</t>
+  </si>
+  <si>
+    <t>(-0.04703740155924357+0.001898673983909183j)</t>
+  </si>
+  <si>
+    <t>(-0.04499750377027421+0.0017890986588416976j)</t>
+  </si>
+  <si>
+    <t>(-0.03976349725342284+0.0015290958625692607j)</t>
+  </si>
+  <si>
+    <t>(-0.06616457923998027+0.0010798198680139273j)</t>
+  </si>
+  <si>
+    <t>(0.0074113187772674735+0.0007307968174368297j)</t>
+  </si>
+  <si>
+    <t>(-0.020776028220721443+0.0008308670030526331j)</t>
+  </si>
+  <si>
+    <t>(-0.06065773722363775+0.0013159591499439364j)</t>
+  </si>
+  <si>
+    <t>(-0.0873297308874979+0.0018066216777757763j)</t>
+  </si>
+  <si>
+    <t>(-0.09197613327926288+0.00194092742374168j)</t>
+  </si>
+  <si>
+    <t>(-0.024915275414023785+0.0006307093886217861j)</t>
+  </si>
+  <si>
+    <t>(-0.05202675750269418+0.001087216161300304j)</t>
+  </si>
+  <si>
+    <t>(0.009310173592267424-0.00017663541091755982j)</t>
+  </si>
+  <si>
+    <t>(0.013294068019233232-0.00029659812162910037j)</t>
+  </si>
+  <si>
+    <t>(0.02357693906904777-0.0005125191095588004j)</t>
+  </si>
+  <si>
+    <t>(-0.0491262142713294+0.0004161256173218924j)</t>
+  </si>
+  <si>
+    <t>(0.06176497092456266+0.00015015887740568365j)</t>
+  </si>
+  <si>
+    <t>(0.019284877244638156+0.0002410331221856428j)</t>
+  </si>
+  <si>
+    <t>(-0.040311555734392365+0.0003252909619827673j)</t>
+  </si>
+  <si>
+    <t>(-0.07987921794206523+0.0003470886806513844j)</t>
+  </si>
+  <si>
+    <t>(-0.08657435363960134+0.00023740449408289936j)</t>
+  </si>
+  <si>
+    <t>(0.012715100055879449+0.00017995911562675585j)</t>
+  </si>
+  <si>
+    <t>(-0.027393745746858503+4.2205865596538463e-05j)</t>
+  </si>
+  <si>
+    <t>(0.06274898820795233+0.00041227183720179993j)</t>
+  </si>
+  <si>
+    <t>(0.06840823370175043+0.0005107907507402509j)</t>
+  </si>
+  <si>
+    <t>(0.08338638206029306+0.0006570078394684941j)</t>
+  </si>
+  <si>
+    <t>(-0.03224318612203692-0.000462402881166388j)</t>
+  </si>
+  <si>
+    <t>(0.11538326195197794+0.0001373168002355836j)</t>
+  </si>
+  <si>
+    <t>(0.05850411113502743+0.00016314293938934378j)</t>
+  </si>
+  <si>
+    <t>(-0.02057600113296159-0.00045532765650903436j)</t>
+  </si>
+  <si>
+    <t>(-0.07278020539508102-0.0011351276778005428j)</t>
+  </si>
+  <si>
+    <t>(-0.08150398409094534-0.0014725548529616874j)</t>
+  </si>
+  <si>
+    <t>(0.04866806093168778+0.0007764918970993878j)</t>
+  </si>
+  <si>
+    <t>(-0.00403899274462911-0.00026327236467428924j)</t>
+  </si>
+  <si>
+    <t>(0.11337688762556684+0.0027749347787422328j)</t>
+  </si>
+  <si>
+    <t>(0.12046370871606427+0.0032227452964180103j)</t>
+  </si>
+  <si>
+    <t>(0.13979887007016226+0.003931048834764423j)</t>
+  </si>
+  <si>
+    <t>(-0.10117585933941962+0.0011341622895107968j)</t>
+  </si>
+  <si>
+    <t>(-0.10331076642550893+0.0031555218653327396j)</t>
+  </si>
+  <si>
+    <t>(-0.10344656700043693+0.003777427406742958j)</t>
+  </si>
+  <si>
+    <t>(-0.10350609458356869+0.004281099291564212j)</t>
+  </si>
+  <si>
+    <t>(-0.1037773423432795+0.004891545257562298j)</t>
+  </si>
+  <si>
+    <t>(-0.10426267505897212+0.005626412219920983j)</t>
+  </si>
+  <si>
+    <t>(-0.10532085855341239+0.006801523233711149j)</t>
+  </si>
+  <si>
+    <t>(-0.10539685112135548+0.0071140452374708375j)</t>
+  </si>
+  <si>
+    <t>(-0.10609794474801805+0.00791434314559838j)</t>
+  </si>
+  <si>
+    <t>(-0.10626045817875548+0.00818805256632607j)</t>
+  </si>
+  <si>
+    <t>(-0.10639771414568566+0.008375889927315801j)</t>
+  </si>
+  <si>
+    <t>(-0.07918929328232452+0.00124856138733727j)</t>
+  </si>
+  <si>
+    <t>(-0.033954440778300114+0.0012472353617124232j)</t>
+  </si>
+  <si>
+    <t>(-0.05149747142684819+0.001478225528964093j)</t>
+  </si>
+  <si>
+    <t>(-0.07644149462856056+0.002161105602465484j)</t>
+  </si>
+  <si>
+    <t>(-0.09326181721964054+0.0028801721735644014j)</t>
+  </si>
+  <si>
+    <t>(-0.09634994362768409+0.0032292492521568384j)</t>
+  </si>
+  <si>
+    <t>(-0.05439546783914915+0.001882489947313875j)</t>
+  </si>
+  <si>
+    <t>(-0.0714817156955381+0.002562497677730097j)</t>
+  </si>
+  <si>
+    <t>(-0.03285032837056704+0.0010591511827626157j)</t>
+  </si>
+  <si>
+    <t>(-0.030311026258158704+0.0009418632174847735j)</t>
+  </si>
+  <si>
+    <t>(-0.023800157648105422+0.0006695444071642303j)</t>
+  </si>
+  <si>
+    <t>(-0.05767761530913588+0.0009022517783820984j)</t>
+  </si>
+  <si>
+    <t>(0.03436270270041589+0.00033207285402268383j)</t>
+  </si>
+  <si>
+    <t>(-0.0008148889535143911+0.000477237247801346j)</t>
+  </si>
+  <si>
+    <t>(-0.05040148834903904+0.0008673314919944363j)</t>
+  </si>
+  <si>
+    <t>(-0.08343024199744256+0.001188502631215257j)</t>
+  </si>
+  <si>
+    <t>(-0.08906428284434789+0.001193662060430512j)</t>
+  </si>
+  <si>
+    <t>(-0.005929078801502459+0.00027978550602474484j)</t>
+  </si>
+  <si>
+    <t>(-0.03947178843725996+0.0005120702821297277j)</t>
+  </si>
+  <si>
+    <t>(0.036281496086616155-0.00011992987499398266j)</t>
+  </si>
+  <si>
+    <t>(0.04113988857624692-0.00014103666421153547j)</t>
+  </si>
+  <si>
+    <t>(0.05379000498402894-0.00020285236087953763j)</t>
+  </si>
+  <si>
+    <t>(-0.03644808250472091+0.00031008961368244264j)</t>
+  </si>
+  <si>
+    <t>(0.1015801029104035+0.0004929316093092797j)</t>
+  </si>
+  <si>
+    <t>(0.04856890361667742+0.0005447847268658015j)</t>
+  </si>
+  <si>
+    <t>(-0.025327387348962345+0.00014122027981460652j)</t>
+  </si>
+  <si>
+    <t>(-0.07416677390767554-0.00035742717796950963j)</t>
+  </si>
+  <si>
+    <t>(-0.08230416179832346-0.0006751058996302631j)</t>
+  </si>
+  <si>
+    <t>(0.03994359600376726+0.0008562870459827754j)</t>
+  </si>
+  <si>
+    <t>(-0.009432300236641695+5.323912138978555e-05j)</t>
+  </si>
+  <si>
+    <t>(0.1010595974352085+0.0023321169481698655j)</t>
+  </si>
+  <si>
+    <t>(0.10785032942501915+0.0026804015029905045j)</t>
+  </si>
+  <si>
+    <t>(0.12611080182743975+0.003234982076278204j)</t>
+  </si>
+  <si>
+    <t>(-0.015444062683866808-0.00037995316785078073j)</t>
+  </si>
+  <si>
+    <t>(0.16760390122030655+0.0016817720761441932j)</t>
+  </si>
+  <si>
+    <t>(0.09666218074883709+0.0014757390052906275j)</t>
+  </si>
+  <si>
+    <t>(-0.00113573352005166-0.00018780774710664935j)</t>
+  </si>
+  <si>
+    <t>(-0.0653657914600951-0.0018446363761073156j)</t>
+  </si>
+  <si>
+    <t>(-0.0759676163464063-0.0024768431746103746j)</t>
+  </si>
+  <si>
+    <t>(0.083383375257526+0.0028454970934043166j)</t>
+  </si>
+  <si>
+    <t>(0.01879273884781598+0.0005909690135617383j)</t>
+  </si>
+  <si>
+    <t>(0.16178580726796918+0.007058235913160554j)</t>
+  </si>
+  <si>
+    <t>(0.17016864568995338+0.007917636974789304j)</t>
+  </si>
+  <si>
+    <t>(0.19355793559011894+0.009324512528884499j)</t>
+  </si>
+  <si>
+    <t>(-0.10113856205969102+0.001225171593319577j)</t>
+  </si>
+  <si>
+    <t>(-0.10310569439709305+0.003146326252627967j)</t>
+  </si>
+  <si>
+    <t>(-0.10336981393730062+0.0038054820771296852j)</t>
+  </si>
+  <si>
+    <t>(-0.10354140051634748+0.004347853412999759j)</t>
+  </si>
+  <si>
+    <t>(-0.10387428318535538+0.004974982173088113j)</t>
+  </si>
+  <si>
+    <t>(-0.10437977047438098+0.005701103449036971j)</t>
+  </si>
+  <si>
+    <t>(-0.10539567522702507+0.006802250748620381j)</t>
+  </si>
+  <si>
+    <t>(-0.10551188439366314+0.007125829172105498j)</t>
+  </si>
+  <si>
+    <t>(-0.10619770484922564+0.007861104956349245j)</t>
+  </si>
+  <si>
+    <t>(-0.10637381648975647+0.008122159270556805j)</t>
+  </si>
+  <si>
+    <t>(-0.10651525367530078+0.008296105108624306j)</t>
+  </si>
+  <si>
+    <t>(-0.07502794272722013+0.0010097178357315949j)</t>
+  </si>
+  <si>
+    <t>(-0.020234894383674817+0.0005865197682651101j)</t>
+  </si>
+  <si>
+    <t>(-0.0413589786603021+0.000921061987994776j)</t>
+  </si>
+  <si>
+    <t>(-0.07133090751434021+0.0017102210494805198j)</t>
+  </si>
+  <si>
+    <t>(-0.09146406119426595+0.0024531696580361202j)</t>
+  </si>
+  <si>
+    <t>(-0.09507246051471938+0.0027498459043748024j)</t>
+  </si>
+  <si>
+    <t>(-0.044680554467879906+0.0012779232205451126j)</t>
+  </si>
+  <si>
+    <t>(-0.06513725147978482+0.001964493735060998j)</t>
+  </si>
+  <si>
+    <t>(-0.01889774278125794+0.00048323618238549116j)</t>
+  </si>
+  <si>
+    <t>(-0.01588336538344388+0.00039360734675150915j)</t>
+  </si>
+  <si>
+    <t>(-0.008114704056948759+0.00014914800772684582j)</t>
+  </si>
+  <si>
+    <t>(-0.049330894188472973+0.0006025397750774289j)</t>
+  </si>
+  <si>
+    <t>(0.06118494869776032-4.1321440635507946e-05j)</t>
+  </si>
+  <si>
+    <t>(0.01891721280049349+0.00020521833222180157j)</t>
+  </si>
+  <si>
+    <t>(-0.04039734084264441+0.0004647677372159821j)</t>
+  </si>
+  <si>
+    <t>(-0.07976361264078646+0.0005682769075180465j)</t>
+  </si>
+  <si>
+    <t>(-0.08638465315773707+0.00045373701779941977j)</t>
+  </si>
+  <si>
+    <t>(0.01257731111798473+0.0002821738536787024j)</t>
+  </si>
+  <si>
+    <t>(-0.027333759616810283+0.00020091812658763023j)</t>
+  </si>
+  <si>
+    <t>(0.06251129704121036+0.0005789862612096097j)</t>
+  </si>
+  <si>
+    <t>(0.06817876956960385+0.0007183043329478425j)</t>
+  </si>
+  <si>
+    <t>(0.08311640599495135+0.0008922130581486736j)</t>
+  </si>
+  <si>
+    <t>(-0.023954696016830465+0.00020022683743411437j)</t>
+  </si>
+  <si>
+    <t>(0.14094875518851369+0.0011179255672313362j)</t>
+  </si>
+  <si>
+    <t>(0.07734095632120334+0.0011560298132858033j)</t>
+  </si>
+  <si>
+    <t>(-0.01074288737972526+0.0001656581545837986j)</t>
+  </si>
+  <si>
+    <t>(-0.06872097529816079-0.0009467373325846814j)</t>
+  </si>
+  <si>
+    <t>(-0.07828201380874882-0.0014663293598872256j)</t>
+  </si>
+  <si>
+    <t>(0.0662715586446652+0.0021444216868551635j)</t>
+  </si>
+  <si>
+    <t>(0.007836262443137662+0.0005354960426571392j)</t>
+  </si>
+  <si>
+    <t>(0.13793592990515507+0.005231312766917542j)</t>
+  </si>
+  <si>
+    <t>(0.14574586639196818+0.005900497106293868j)</t>
+  </si>
+  <si>
+    <t>(0.16712813908211485+0.0069665466742382985j)</t>
+  </si>
+  <si>
+    <t>(0.001100517649549942-9.142291484480984e-05j)</t>
+  </si>
+  <si>
+    <t>(0.21892370217540336+0.003819028807490672j)</t>
+  </si>
+  <si>
+    <t>(0.13392737858243228+0.0033703549985291256j)</t>
+  </si>
+  <si>
+    <t>(0.017720034672825416+0.0005121277118719716j)</t>
+  </si>
+  <si>
+    <t>(-0.058247909029480766-0.0022474759853626015j)</t>
+  </si>
+  <si>
+    <t>(-0.07068344191425385-0.0031730643865657024j)</t>
+  </si>
+  <si>
+    <t>(0.11669563936854849+0.005782104440387202j)</t>
+  </si>
+  <si>
+    <t>(0.04061589908026288+0.0021411852509644444j)</t>
+  </si>
+  <si>
+    <t>(0.20795285363442054+0.012592875432462935j)</t>
+  </si>
+  <si>
+    <t>(0.21747348044293666+0.013931080422808264j)</t>
+  </si>
+  <si>
+    <t>(0.244666406200654+0.016143154496794467j)</t>
+  </si>
+  <si>
+    <t>(-0.10109626215927983+0.0013697784563567713j)</t>
+  </si>
+  <si>
+    <t>(-0.10283820123709937+0.003025367117195747j)</t>
+  </si>
+  <si>
+    <t>(-0.10327219063445094+0.0037962319596872877j)</t>
+  </si>
+  <si>
+    <t>(-0.10358943316221766+0.004460850616715139j)</t>
+  </si>
+  <si>
+    <t>(-0.10400038647841085+0.005152763069261444j)</t>
+  </si>
+  <si>
+    <t>(-0.1045286612958141+0.005873940678819135j)</t>
+  </si>
+  <si>
+    <t>(-0.10547850563407982+0.006781602595522795j)</t>
+  </si>
+  <si>
+    <t>(-0.10564502057045869+0.0071596036115618945j)</t>
+  </si>
+  <si>
+    <t>(-0.10629503180717324+0.007726232983613446j)</t>
+  </si>
+  <si>
+    <t>(-0.10648271747935693+0.007966608788214626j)</t>
+  </si>
+  <si>
+    <t>(-0.10662429916022967+0.00810906649833741j)</t>
+  </si>
+  <si>
+    <t>(-0.07094500302970383+0.0006700801964488359j)</t>
+  </si>
+  <si>
+    <t>(-0.006470308282021249-0.00017088833949322277j)</t>
+  </si>
+  <si>
+    <t>(-0.03126547317786923+0.0003268666513348737j)</t>
+  </si>
+  <si>
+    <t>(-0.06633996531566708+0.0012410638100780538j)</t>
+  </si>
+  <si>
+    <t>(-0.08982036604726963+0.002005355286277322j)</t>
+  </si>
+  <si>
+    <t>(-0.09395633533038333+0.002257150333819507j)</t>
+  </si>
+  <si>
+    <t>(-0.03513111618490159+0.0007883686002406879j)</t>
+  </si>
+  <si>
+    <t>(-0.05897393137156034+0.001455705144723554j)</t>
+  </si>
+  <si>
+    <t>(-0.005175608050274408+0.0001520411219205888j)</t>
+  </si>
+  <si>
+    <t>(-0.0017101291943271723+0.0001211231745143266j)</t>
+  </si>
+  <si>
+    <t>(0.00729618354241966-5.871744782564584e-05j)</t>
+  </si>
+  <si>
+    <t>(-0.041103956468166634+0.00019455616088091953j)</t>
+  </si>
+  <si>
+    <t>(0.0878923995533116-0.0003754429744318001j)</t>
+  </si>
+  <si>
+    <t>(0.03843999940574797+1.179370946298295e-05j)</t>
+  </si>
+  <si>
+    <t>(-0.030623141252568802+9.974682417856749e-05j)</t>
+  </si>
+  <si>
+    <t>(-0.07630823077147113-6.179591748718256e-05j)</t>
+  </si>
+  <si>
+    <t>(-0.08391654426342256-0.00028850037926873937j)</t>
+  </si>
+  <si>
+    <t>(0.030633185903799952+0.0005916068554343801j)</t>
+  </si>
+  <si>
+    <t>(-0.015586004248958115+0.00011477074781098692j)</t>
+  </si>
+  <si>
+    <t>(0.08804070477319056+0.0018355923999402784j)</t>
+  </si>
+  <si>
+    <t>(0.0944552092341157+0.002187482250009264j)</t>
+  </si>
+  <si>
+    <t>(0.11160463102779312+0.002667731516640223j)</t>
+  </si>
+  <si>
+    <t>(-0.011630355859645109+8.786327499933958e-05j)</t>
+  </si>
+  <si>
+    <t>(0.1798933175922811+0.001987835415294721j)</t>
+  </si>
+  <si>
+    <t>(0.10563553027120254+0.002027159504104397j)</t>
+  </si>
+  <si>
+    <t>(0.0034734514390796284+0.000364243486753876j)</t>
+  </si>
+  <si>
+    <t>(-0.06351865396390353-0.001439532368025645j)</t>
+  </si>
+  <si>
+    <t>(-0.07448695809514674-0.0021547929230308445j)</t>
+  </si>
+  <si>
+    <t>(0.09176886962837634+0.003939034706544554j)</t>
+  </si>
+  <si>
+    <t>(0.02446603653622157+0.0014091286086610174j)</t>
+  </si>
+  <si>
+    <t>(0.17349274576024595+0.008935273580908037j)</t>
+  </si>
+  <si>
+    <t>(0.18221980241522118+0.00998236171044242j)</t>
+  </si>
+  <si>
+    <t>(0.2065772833685739+0.01164299543162779j)</t>
+  </si>
+  <si>
+    <t>(0.017397724884850585+0.0003811779489618428j)</t>
+  </si>
+  <si>
+    <t>(0.26937237642359374+0.006437325913168453j)</t>
+  </si>
+  <si>
+    <t>(0.17035311857783783+0.0057377877682437345j)</t>
+  </si>
+  <si>
+    <t>(0.0360359872877287+0.0015748738229222244j)</t>
+  </si>
+  <si>
+    <t>(-0.051399927847480924-0.0023777495206918292j)</t>
+  </si>
+  <si>
+    <t>(-0.06562832051486332-0.0035916738361511736j)</t>
+  </si>
+  <si>
+    <t>(0.1487317002656694+0.009411469094252686j)</t>
+  </si>
+  <si>
+    <t>(0.06152409266820897+0.0042607731388139385j)</t>
+  </si>
+  <si>
+    <t>(0.25209455776045386+0.019103571282533073j)</t>
+  </si>
+  <si>
+    <t>(0.26261409335811847+0.020970000781092228j)</t>
+  </si>
+  <si>
+    <t>(0.2933873867917366+0.02406483355342968j)</t>
+  </si>
+  <si>
+    <t>(-0.10105518507296991+0.0015686396818661852j)</t>
+  </si>
+  <si>
+    <t>(-0.10254556622663637+0.0028092985717445584j)</t>
+  </si>
+  <si>
+    <t>(-0.10317021617532278+0.0037560607156098946j)</t>
+  </si>
+  <si>
+    <t>(-0.10364756169778858+0.004618330120691686j)</t>
+  </si>
+  <si>
+    <t>(-0.10414256383724105+0.005419697392916077j)</t>
+  </si>
+  <si>
+    <t>(-0.10469361526430766+0.006139844828291873j)</t>
+  </si>
+  <si>
+    <t>(-0.10556416479164209+0.006739359207366818j)</t>
+  </si>
+  <si>
+    <t>(-0.10578376263608025+0.007213709427416518j)</t>
+  </si>
+  <si>
+    <t>(-0.1063820634006242+0.007510762322217612j)</t>
+  </si>
+  <si>
+    <t>(-0.10657704656715325+0.007722605910729245j)</t>
+  </si>
+  <si>
+    <t>(-0.1067141949856758+0.007816351165947526j)</t>
+  </si>
+  <si>
+    <t>(-0.06692818677342498+0.00024156325937399803j)</t>
+  </si>
+  <si>
+    <t>(0.00733368806852656-0.0009968715801409623j)</t>
+  </si>
+  <si>
+    <t>(-0.02121462409521329-0.000290316661961403j)</t>
+  </si>
+  <si>
+    <t>(-0.06145679145804867+0.0007566922778074006j)</t>
+  </si>
+  <si>
+    <t>(-0.08831316851326906+0.0015346863307472139j)</t>
+  </si>
+  <si>
+    <t>(-0.09298319757075255+0.0017474489878151118j)</t>
+  </si>
+  <si>
+    <t>(-0.025740168454171156+0.00040682696229419024j)</t>
+  </si>
+  <si>
+    <t>(-0.05297963179694954+0.0010271248609110314j)</t>
+  </si>
+  <si>
+    <t>(0.008320237224226732+4.7509911782645244e-05j)</t>
+  </si>
+  <si>
+    <t>(0.01221334969990386+0.00010269284803924686j)</t>
+  </si>
+  <si>
+    <t>(0.0224364684805689+2.1073372538082712e-05j)</t>
+  </si>
+  <si>
+    <t>(-0.032980514745155926-0.0003094831985286351j)</t>
+  </si>
+  <si>
+    <t>(0.11449517906407608-0.0006578635504874013j)</t>
+  </si>
+  <si>
+    <t>(0.05776942467112001-0.00010479773086114155j)</t>
+  </si>
+  <si>
+    <t>(-0.021059989838958067-0.00023422780622879422j)</t>
+  </si>
+  <si>
+    <t>(-0.07304523834953844-0.0007077245345830419j)</t>
+  </si>
+  <si>
+    <t>(-0.08164163891238728-0.0010407167484156425j)</t>
+  </si>
+  <si>
+    <t>(0.04826489660021997+0.001170492429837773j)</t>
+  </si>
+  <si>
+    <t>(-0.004204268132812831+0.00022190498120672756j)</t>
+  </si>
+  <si>
+    <t>(0.11290740478245373+0.0035810261231232917j)</t>
+  </si>
+  <si>
+    <t>(0.12001013563690732+0.00418994381747777j)</t>
+  </si>
+  <si>
+    <t>(0.13929933796320415+0.005038183989254528j)</t>
+  </si>
+  <si>
+    <t>(0.000538359344671113-2.565004202798724e-05j)</t>
+  </si>
+  <si>
+    <t>(0.2184365771766974+0.003074967821412182j)</t>
+  </si>
+  <si>
+    <t>(0.13348446870039612+0.0031222345670418243j)</t>
+  </si>
+  <si>
+    <t>(0.0173492382667093+0.0007105404547026624j)</t>
+  </si>
+  <si>
+    <t>(-0.0585403331501077-0.001850833687744307j)</t>
+  </si>
+  <si>
+    <t>(-0.07090142780098878-0.0027556994178568554j)</t>
+  </si>
+  <si>
+    <t>(0.1164976191993877+0.0061595416530418525j)</t>
+  </si>
+  <si>
+    <t>(0.040504689437200536+0.0026123859497719916j)</t>
+  </si>
+  <si>
+    <t>(0.20783164723543257+0.01331101345788614j)</t>
+  </si>
+  <si>
+    <t>(0.21738252830747062+0.014782273440687888j)</t>
+  </si>
+  <si>
+    <t>(0.24458081264176762+0.01710555404748996j)</t>
+  </si>
+  <si>
+    <t>(0.03345570590546598+0.0010189217148014811j)</t>
+  </si>
+  <si>
+    <t>(0.3189890713174064+0.009449795027101606j)</t>
+  </si>
+  <si>
+    <t>(0.20599260985601386+0.008494690034158888j)</t>
+  </si>
+  <si>
+    <t>(0.0538514853624095+0.002946935821489403j)</t>
+  </si>
+  <si>
+    <t>(-0.04480150481552657-0.002262948314159235j)</t>
+  </si>
+  <si>
+    <t>(-0.060785460552525976-0.0037577577012413033j)</t>
+  </si>
+  <si>
+    <t>(0.17960256557716608+0.013604127045341922j)</t>
+  </si>
+  <si>
+    <t>(0.08159714646351103+0.006855000183843875j)</t>
+  </si>
+  <si>
+    <t>(0.2943989152248199+0.026389234604060445j)</t>
+  </si>
+  <si>
+    <t>(0.30579440774895356+0.028820788559516745j)</t>
+  </si>
+  <si>
+    <t>(0.33994809919047925+0.03285532714694568j)</t>
+  </si>
+  <si>
+    <t>(-0.1010204743604085+0.0018206926587592176j)</t>
+  </si>
+  <si>
+    <t>(-0.10225371422289806+0.0025050827391384554j)</t>
+  </si>
+  <si>
+    <t>(-0.10307534452216675+0.003687179585156421j)</t>
+  </si>
+  <si>
+    <t>(-0.10371435830371498+0.0048189299323075484j)</t>
+  </si>
+  <si>
+    <t>(-0.10429254421560072+0.005773149175266567j)</t>
+  </si>
+  <si>
+    <t>(-0.10486463639833453+0.006496626059664537j)</t>
+  </si>
+  <si>
+    <t>(-0.10564868903797334+0.006676497944414568j)</t>
+  </si>
+  <si>
+    <t>(-0.10591966045233682+0.0072887855902374205j)</t>
+  </si>
+  <si>
+    <t>(-0.10645241076398371+0.007217896357925821j)</t>
+  </si>
+  <si>
+    <t>(-0.10664884768653819+0.007394009308396741j)</t>
+  </si>
+  <si>
+    <t>(-0.10677645482027329+0.007422449598075717j)</t>
+  </si>
+  <si>
+    <t>(-0.06296775675951731-0.0002657505491048026j)</t>
+  </si>
+  <si>
+    <t>(0.021171363946941215-0.0018699014619940235j)</t>
+  </si>
+  <si>
+    <t>(-0.011204992951782157-0.0009199429364619079j)</t>
+  </si>
+  <si>
+    <t>(-0.056671628925695175+0.0002595797898144244j)</t>
+  </si>
+  <si>
+    <t>(-0.0869278292642797+0.0010401093143046472j)</t>
+  </si>
+  <si>
+    <t>(-0.09213768783677902+0.0012184157181333332j)</t>
+  </si>
+  <si>
+    <t>(-0.016501546007751042+0.00012639502286933087j)</t>
+  </si>
+  <si>
+    <t>(-0.047143903523991344+0.0006709285836997528j)</t>
+  </si>
+  <si>
+    <t>(0.021594140532438466+0.0001526380709413288j)</t>
+  </si>
+  <si>
+    <t>(0.025891998633453647+0.00031817604644309187j)</t>
+  </si>
+  <si>
+    <t>(0.03731064907572266+0.00036548817734877046j)</t>
+  </si>
+  <si>
+    <t>(-0.02494737656677968-0.0008988105096598229j)</t>
+  </si>
+  <si>
+    <t>(0.14100034169808867-0.0008775891688519979j)</t>
+  </si>
+  <si>
+    <t>(0.07691852054046601-0.00014552863132262018j)</t>
+  </si>
+  <si>
+    <t>(-0.011691610889108273-0.0005421809162986326j)</t>
+  </si>
+  <si>
+    <t>(-0.06995804223526417-0.0013742035491748129j)</t>
+  </si>
+  <si>
+    <t>(-0.07954363265541808-0.0018090363610742534j)</t>
+  </si>
+  <si>
+    <t>(0.06549603249129986+0.0019878332399593576j)</t>
+  </si>
+  <si>
+    <t>(0.006833382710812897+0.0004961675697263033j)</t>
+  </si>
+  <si>
+    <t>(0.13714554785868047+0.005758333559394403j)</t>
+  </si>
+  <si>
+    <t>(0.14488074020580627+0.006662364809513913j)</t>
+  </si>
+  <si>
+    <t>(0.1662411376125751+0.007932822355116083j)</t>
+  </si>
+  <si>
+    <t>(0.01256305176848074-0.00013887094140975492j)</t>
+  </si>
+  <si>
+    <t>(0.2566002952955844+0.004358991106225487j)</t>
+  </si>
+  <si>
+    <t>(0.1609164563318475+0.004413923064551251j)</t>
+  </si>
+  <si>
+    <t>(0.030908562928862213+0.001183875170094029j)</t>
+  </si>
+  <si>
+    <t>(-0.053769421123190664-0.002192991239744409j)</t>
+  </si>
+  <si>
+    <t>(-0.06751045019766326-0.0032817959428194255j)</t>
+  </si>
+  <si>
+    <t>(0.1405122257828167+0.008743134839978378j)</t>
+  </si>
+  <si>
+    <t>(0.05599384838855715+0.004096555587180381j)</t>
+  </si>
+  <si>
+    <t>(0.2410413352316934+0.018255239674937963j)</t>
+  </si>
+  <si>
+    <t>(0.2513302658483894+0.02018858151521081j)</t>
+  </si>
+  <si>
+    <t>(0.2812454751576078+0.023230994852973794j)</t>
+  </si>
+  <si>
+    <t>(0.0492830215885258+0.0018057296549812399j)</t>
+  </si>
+  <si>
+    <t>(0.3678165690588087+0.012789361415029583j)</t>
+  </si>
+  <si>
+    <t>(0.24089621595254682+0.011577055435536106j)</t>
+  </si>
+  <si>
+    <t>(0.07120080249405114+0.004586426144633176j)</t>
+  </si>
+  <si>
+    <t>(-0.0384368844160583-0.0019260066660607275j)</t>
+  </si>
+  <si>
+    <t>(-0.05614249900875132-0.003692755234608636j)</t>
+  </si>
+  <si>
+    <t>(0.2094039341292154+0.018262371655100543j)</t>
+  </si>
+  <si>
+    <t>(0.10090255082953287+0.009851280174183352j)</t>
+  </si>
+  <si>
+    <t>(0.3350268718340239+0.0343001284143412j)</t>
+  </si>
+  <si>
+    <t>(0.34718841615372126+0.03732465611943532j)</t>
+  </si>
+  <si>
+    <t>(0.38454223906901075+0.04234096319143914j)</t>
+  </si>
+  <si>
+    <t>(-0.10099620306909837+0.0021238267001463603j)</t>
+  </si>
+  <si>
+    <t>(-0.10197959616484747+0.002113984965151653j)</t>
+  </si>
+  <si>
+    <t>(-0.10299503052061251+0.0035893245848731894j)</t>
+  </si>
+  <si>
+    <t>(-0.10378921622817447+0.005061421751331855j)</t>
+  </si>
+  <si>
+    <t>(-0.10444559461114339+0.006211802777733115j)</t>
+  </si>
+  <si>
+    <t>(-0.10503594693281758+0.006943558451942423j)</t>
+  </si>
+  <si>
+    <t>(-0.10572918085251756+0.006594500077959895j)</t>
+  </si>
+  <si>
+    <t>(-0.10604736984559465+0.007386526822486757j)</t>
+  </si>
+  <si>
+    <t>(-0.10650116473123411+0.006851792152194242j)</t>
+  </si>
+  <si>
+    <t>(-0.10669220079081501+0.006985854618522442j)</t>
+  </si>
+  <si>
+    <t>(-0.10680470092819071+0.0069331475490920945j)</t>
+  </si>
+  <si>
+    <t>(-0.05905581567312695-0.0008432719206465958j)</t>
+  </si>
+  <si>
+    <t>(0.035037370393712304-0.0027732667310628374j)</t>
+  </si>
+  <si>
+    <t>(-0.001235570230403035-0.0015540149684984505j)</t>
+  </si>
+  <si>
+    <t>(-0.051976294198512234-0.00024828041193911436j)</t>
+  </si>
+  <si>
+    <t>(-0.08565201414712381+0.0005211822465912234j)</t>
+  </si>
+  <si>
+    <t>(-0.09140684569716775+0.0006686233325957533j)</t>
+  </si>
+  <si>
+    <t>(-0.007409665535816607-5.9600615764799805e-05j)</t>
+  </si>
+  <si>
+    <t>(-0.04145762191872127+0.00038022782730082346j)</t>
+  </si>
+  <si>
+    <t>(0.03465061514106603+0.00045155050330785443j)</t>
+  </si>
+  <si>
+    <t>(0.03933094079083767+0.000748983658328169j)</t>
+  </si>
+  <si>
+    <t>(0.051923624527799146+0.0009532976605466174j)</t>
+  </si>
+  <si>
+    <t>(-0.016993699387955946-0.0015638935509643297j)</t>
+  </si>
+  <si>
+    <t>(0.16741265848705508-0.0010249323924945797j)</t>
+  </si>
+  <si>
+    <t>(0.09589801495931481-0.0001108778985736917j)</t>
+  </si>
+  <si>
+    <t>(-0.0025038701797163465-0.0008280422405626685j)</t>
+  </si>
+  <si>
+    <t>(-0.06703193159246269-0.0020649069833608845j)</t>
+  </si>
+  <si>
+    <t>(-0.07760793053546168-0.002598364543781636j)</t>
+  </si>
+  <si>
+    <t>(0.08234768909944387+0.003017713535601308j)</t>
+  </si>
+  <si>
+    <t>(0.017546751917000364+0.0009157301889188162j)</t>
+  </si>
+  <si>
+    <t>(0.16078594281951655+0.008319737540995515j)</t>
+  </si>
+  <si>
+    <t>(0.1691006486645021+0.009551617841904775j)</t>
+  </si>
+  <si>
+    <t>(0.1924667638818499+0.011292278262049751j)</t>
+  </si>
+  <si>
+    <t>(0.024453816224239096-0.00025024749550904015j)</t>
+  </si>
+  <si>
+    <t>(0.29440449422695064+0.0058251472274276975j)</t>
+  </si>
+  <si>
+    <t>(0.18795697310564913+0.005881263944789226j)</t>
+  </si>
+  <si>
+    <t>(0.04417243852899489+0.0017678201306599284j)</t>
+  </si>
+  <si>
+    <t>(-0.04919160432060662-0.0024763493083666886j)</t>
+  </si>
+  <si>
+    <t>(-0.06430106969157905-0.003743952243714388j)</t>
+  </si>
+  <si>
+    <t>(0.16386013555694434+0.011639942595124067j)</t>
+  </si>
+  <si>
+    <t>(0.07096979111790161+0.005822462568560146j)</t>
+  </si>
+  <si>
+    <t>(0.27319885180102293+0.023686133155520137j)</t>
+  </si>
+  <si>
+    <t>(0.28414649572317313+0.02611280305715146j)</t>
+  </si>
+  <si>
+    <t>(0.3166638084872472+0.029921737539384863j)</t>
+  </si>
+  <si>
+    <t>(0.0648882401866887+0.002728032758049538j)</t>
+  </si>
+  <si>
+    <t>(0.415897916832626+0.01640447786855638j)</t>
+  </si>
+  <si>
+    <t>(0.2751103057429707+0.014935376065542594j)</t>
+  </si>
+  <si>
+    <t>(0.0881136553306987+0.006459932611999707j)</t>
+  </si>
+  <si>
+    <t>(-0.03229366538583812-0.0013865993811921452j)</t>
+  </si>
+  <si>
+    <t>(-0.05169016672378711-0.003415505356008665j)</t>
+  </si>
+  <si>
+    <t>(0.23821783714803524+0.023310977905417075j)</t>
+  </si>
+  <si>
+    <t>(0.11949729009476118+0.013192645349560375j)</t>
+  </si>
+  <si>
+    <t>(0.3741155357554581+0.042722454359650296j)</t>
+  </si>
+  <si>
+    <t>(0.3869439314342349+0.046361064562615836j)</t>
+  </si>
+  <si>
+    <t>(0.42733422524956405+0.05239023805108316j)</t>
   </si>
 </sst>
 </file>

</xml_diff>